<commit_message>
prep word lists for Susanne
</commit_message>
<xml_diff>
--- a/data/word_list_5.xlsx
+++ b/data/word_list_5.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K345"/>
+  <dimension ref="A1:G345"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -365,52 +365,32 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>select</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>aoa_german_comb</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>word_freq</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>aoa_german_b_m</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>aoa_german_s_m</t>
-        </is>
-      </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>aoa_german_l_m</t>
+          <t>aoa_mor</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>aoa_german_comb</t>
+          <t>clt</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>clt</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
           <t>english</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>aoa_mor</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>aoa_rating_english</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>select</t>
         </is>
       </c>
     </row>
@@ -423,10 +403,7 @@
       <c r="C2">
         <v>6.38</v>
       </c>
-      <c r="F2">
-        <v>6.38</v>
-      </c>
-      <c r="H2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>spare time</t>
         </is>
@@ -441,10 +418,7 @@
       <c r="C3">
         <v>6.38</v>
       </c>
-      <c r="F3">
-        <v>6.38</v>
-      </c>
-      <c r="H3" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>poppy</t>
         </is>
@@ -459,10 +433,7 @@
       <c r="C4">
         <v>6.38</v>
       </c>
-      <c r="F4">
-        <v>6.38</v>
-      </c>
-      <c r="H4" t="inlineStr">
+      <c r="G4" t="inlineStr">
         <is>
           <t>rascal</t>
         </is>
@@ -477,10 +448,7 @@
       <c r="C5">
         <v>6.38</v>
       </c>
-      <c r="F5">
-        <v>6.38</v>
-      </c>
-      <c r="H5" t="inlineStr">
+      <c r="G5" t="inlineStr">
         <is>
           <t>thousand</t>
         </is>
@@ -495,10 +463,7 @@
       <c r="C6">
         <v>6.38</v>
       </c>
-      <c r="F6">
-        <v>6.38</v>
-      </c>
-      <c r="H6" t="inlineStr">
+      <c r="G6" t="inlineStr">
         <is>
           <t>fool</t>
         </is>
@@ -513,10 +478,7 @@
       <c r="C7">
         <v>6.38</v>
       </c>
-      <c r="F7">
-        <v>6.38</v>
-      </c>
-      <c r="H7" t="inlineStr">
+      <c r="G7" t="inlineStr">
         <is>
           <t>detour</t>
         </is>
@@ -531,10 +493,7 @@
       <c r="C8">
         <v>6.39</v>
       </c>
-      <c r="F8">
-        <v>6.39</v>
-      </c>
-      <c r="H8" t="inlineStr">
+      <c r="G8" t="inlineStr">
         <is>
           <t>juggle</t>
         </is>
@@ -549,10 +508,7 @@
       <c r="C9">
         <v>6.39</v>
       </c>
-      <c r="F9">
-        <v>6.39</v>
-      </c>
-      <c r="H9" t="inlineStr">
+      <c r="G9" t="inlineStr">
         <is>
           <t>oaf</t>
         </is>
@@ -567,10 +523,7 @@
       <c r="C10">
         <v>6.4</v>
       </c>
-      <c r="F10">
-        <v>6.4</v>
-      </c>
-      <c r="H10" t="inlineStr">
+      <c r="G10" t="inlineStr">
         <is>
           <t>distance</t>
         </is>
@@ -585,10 +538,7 @@
       <c r="C11">
         <v>6.4</v>
       </c>
-      <c r="F11">
-        <v>6.4</v>
-      </c>
-      <c r="H11" t="inlineStr">
+      <c r="G11" t="inlineStr">
         <is>
           <t>explosion</t>
         </is>
@@ -603,10 +553,7 @@
       <c r="C12">
         <v>6.4</v>
       </c>
-      <c r="F12">
-        <v>6.4</v>
-      </c>
-      <c r="H12" t="inlineStr">
+      <c r="G12" t="inlineStr">
         <is>
           <t>rogue</t>
         </is>
@@ -621,10 +568,7 @@
       <c r="C13">
         <v>6.4</v>
       </c>
-      <c r="F13">
-        <v>6.4</v>
-      </c>
-      <c r="H13" t="inlineStr">
+      <c r="G13" t="inlineStr">
         <is>
           <t>hint</t>
         </is>
@@ -639,10 +583,7 @@
       <c r="C14">
         <v>6.4</v>
       </c>
-      <c r="F14">
-        <v>6.4</v>
-      </c>
-      <c r="H14" t="inlineStr">
+      <c r="G14" t="inlineStr">
         <is>
           <t>cheering</t>
         </is>
@@ -657,10 +598,7 @@
       <c r="C15">
         <v>6.4</v>
       </c>
-      <c r="F15">
-        <v>6.4</v>
-      </c>
-      <c r="H15" t="inlineStr">
+      <c r="G15" t="inlineStr">
         <is>
           <t>envy</t>
         </is>
@@ -675,19 +613,13 @@
       <c r="C16">
         <v>6.4</v>
       </c>
-      <c r="F16">
-        <v>6.4</v>
-      </c>
-      <c r="H16" t="inlineStr">
+      <c r="E16">
+        <v>3.71</v>
+      </c>
+      <c r="G16" t="inlineStr">
         <is>
           <t>soldier</t>
         </is>
-      </c>
-      <c r="I16">
-        <v>3.71</v>
-      </c>
-      <c r="J16">
-        <v>6.44</v>
       </c>
     </row>
     <row r="17">
@@ -699,10 +631,7 @@
       <c r="C17">
         <v>6.4</v>
       </c>
-      <c r="F17">
-        <v>6.4</v>
-      </c>
-      <c r="H17" t="inlineStr">
+      <c r="G17" t="inlineStr">
         <is>
           <t>grief</t>
         </is>
@@ -714,16 +643,13 @@
           <t>chemieingenieur</t>
         </is>
       </c>
-      <c r="B18">
+      <c r="C18">
+        <v>6.4</v>
+      </c>
+      <c r="D18">
         <v>0.01</v>
       </c>
-      <c r="D18">
-        <v>6.4</v>
-      </c>
-      <c r="F18">
-        <v>6.4</v>
-      </c>
-      <c r="H18" t="inlineStr">
+      <c r="G18" t="inlineStr">
         <is>
           <t>chemical engineer</t>
         </is>
@@ -735,16 +661,13 @@
           <t>heilpraktiker</t>
         </is>
       </c>
-      <c r="B19">
+      <c r="C19">
+        <v>6.4</v>
+      </c>
+      <c r="D19">
         <v>0.24</v>
       </c>
-      <c r="D19">
-        <v>6.4</v>
-      </c>
-      <c r="F19">
-        <v>6.4</v>
-      </c>
-      <c r="H19" t="inlineStr">
+      <c r="G19" t="inlineStr">
         <is>
           <t>healer</t>
         </is>
@@ -756,13 +679,10 @@
           <t>landschaftsgestalter</t>
         </is>
       </c>
-      <c r="D20">
+      <c r="C20">
         <v>6.4</v>
       </c>
-      <c r="F20">
-        <v>6.4</v>
-      </c>
-      <c r="H20" t="inlineStr">
+      <c r="G20" t="inlineStr">
         <is>
           <t>landscape architect</t>
         </is>
@@ -774,16 +694,13 @@
           <t>anwaltsgehilfe</t>
         </is>
       </c>
-      <c r="B21">
+      <c r="C21">
+        <v>6.4</v>
+      </c>
+      <c r="D21">
         <v>0.01</v>
       </c>
-      <c r="D21">
-        <v>6.4</v>
-      </c>
-      <c r="F21">
-        <v>6.4</v>
-      </c>
-      <c r="H21" t="inlineStr">
+      <c r="G21" t="inlineStr">
         <is>
           <t>paralegal</t>
         </is>
@@ -795,16 +712,13 @@
           <t>großhandelskaufmann</t>
         </is>
       </c>
-      <c r="B22">
+      <c r="C22">
+        <v>6.4</v>
+      </c>
+      <c r="D22">
         <v>0.01</v>
       </c>
-      <c r="D22">
-        <v>6.4</v>
-      </c>
-      <c r="F22">
-        <v>6.4</v>
-      </c>
-      <c r="H22" t="inlineStr">
+      <c r="G22" t="inlineStr">
         <is>
           <t>wholesaler</t>
         </is>
@@ -819,10 +733,7 @@
       <c r="C23">
         <v>6.41</v>
       </c>
-      <c r="F23">
-        <v>6.41</v>
-      </c>
-      <c r="H23" t="inlineStr">
+      <c r="G23" t="inlineStr">
         <is>
           <t>jaw</t>
         </is>
@@ -837,10 +748,7 @@
       <c r="C24">
         <v>6.41</v>
       </c>
-      <c r="F24">
-        <v>6.41</v>
-      </c>
-      <c r="H24" t="inlineStr">
+      <c r="G24" t="inlineStr">
         <is>
           <t>rust</t>
         </is>
@@ -852,16 +760,13 @@
           <t>rechtspfleger</t>
         </is>
       </c>
-      <c r="B25">
+      <c r="C25">
+        <v>6.41</v>
+      </c>
+      <c r="D25">
         <v>0.22</v>
       </c>
-      <c r="D25">
-        <v>6.41</v>
-      </c>
-      <c r="F25">
-        <v>6.41</v>
-      </c>
-      <c r="H25" t="inlineStr">
+      <c r="G25" t="inlineStr">
         <is>
           <t>judicial officer</t>
         </is>
@@ -876,10 +781,7 @@
       <c r="C26">
         <v>6.42</v>
       </c>
-      <c r="F26">
-        <v>6.42</v>
-      </c>
-      <c r="H26" t="inlineStr">
+      <c r="G26" t="inlineStr">
         <is>
           <t>escape</t>
         </is>
@@ -894,10 +796,7 @@
       <c r="C27">
         <v>6.42</v>
       </c>
-      <c r="F27">
-        <v>6.42</v>
-      </c>
-      <c r="H27" t="inlineStr">
+      <c r="G27" t="inlineStr">
         <is>
           <t>happen</t>
         </is>
@@ -912,10 +811,7 @@
       <c r="C28">
         <v>6.42</v>
       </c>
-      <c r="F28">
-        <v>6.42</v>
-      </c>
-      <c r="H28" t="inlineStr">
+      <c r="G28" t="inlineStr">
         <is>
           <t>glide</t>
         </is>
@@ -930,10 +826,7 @@
       <c r="C29">
         <v>6.42</v>
       </c>
-      <c r="F29">
-        <v>6.42</v>
-      </c>
-      <c r="H29" t="inlineStr">
+      <c r="G29" t="inlineStr">
         <is>
           <t>lipstick</t>
         </is>
@@ -948,10 +841,7 @@
       <c r="C30">
         <v>6.42</v>
       </c>
-      <c r="F30">
-        <v>6.42</v>
-      </c>
-      <c r="H30" t="inlineStr">
+      <c r="G30" t="inlineStr">
         <is>
           <t>in writing</t>
         </is>
@@ -966,10 +856,7 @@
       <c r="C31">
         <v>6.42</v>
       </c>
-      <c r="F31">
-        <v>6.42</v>
-      </c>
-      <c r="H31" t="inlineStr">
+      <c r="G31" t="inlineStr">
         <is>
           <t>split</t>
         </is>
@@ -984,10 +871,7 @@
       <c r="C32">
         <v>6.42</v>
       </c>
-      <c r="F32">
-        <v>6.42</v>
-      </c>
-      <c r="H32" t="inlineStr">
+      <c r="G32" t="inlineStr">
         <is>
           <t>whisper to</t>
         </is>
@@ -1002,10 +886,7 @@
       <c r="C33">
         <v>6.42</v>
       </c>
-      <c r="F33">
-        <v>6.42</v>
-      </c>
-      <c r="H33" t="inlineStr">
+      <c r="G33" t="inlineStr">
         <is>
           <t>supplies</t>
         </is>
@@ -1017,19 +898,13 @@
           <t>aal</t>
         </is>
       </c>
-      <c r="B34">
-        <v>3.2</v>
-      </c>
       <c r="C34">
         <v>6.43</v>
       </c>
       <c r="D34">
-        <v>3.05</v>
-      </c>
-      <c r="F34">
-        <v>6.43</v>
-      </c>
-      <c r="H34" t="inlineStr">
+        <v>3.2</v>
+      </c>
+      <c r="G34" t="inlineStr">
         <is>
           <t>eel</t>
         </is>
@@ -1044,10 +919,7 @@
       <c r="C35">
         <v>6.43</v>
       </c>
-      <c r="F35">
-        <v>6.43</v>
-      </c>
-      <c r="H35" t="inlineStr">
+      <c r="G35" t="inlineStr">
         <is>
           <t>departure</t>
         </is>
@@ -1062,10 +934,7 @@
       <c r="C36">
         <v>6.43</v>
       </c>
-      <c r="F36">
-        <v>6.43</v>
-      </c>
-      <c r="H36" t="inlineStr">
+      <c r="G36" t="inlineStr">
         <is>
           <t>factory</t>
         </is>
@@ -1080,10 +949,7 @@
       <c r="C37">
         <v>6.43</v>
       </c>
-      <c r="F37">
-        <v>6.43</v>
-      </c>
-      <c r="H37" t="inlineStr">
+      <c r="G37" t="inlineStr">
         <is>
           <t>miserly</t>
         </is>
@@ -1095,28 +961,19 @@
           <t>richter</t>
         </is>
       </c>
-      <c r="B38">
-        <v>69.22</v>
-      </c>
       <c r="C38">
         <v>6.43</v>
       </c>
       <c r="D38">
-        <v>4.5</v>
-      </c>
-      <c r="F38">
-        <v>6.43</v>
-      </c>
-      <c r="H38" t="inlineStr">
+        <v>69.22</v>
+      </c>
+      <c r="E38">
+        <v>8.539999999999999</v>
+      </c>
+      <c r="G38" t="inlineStr">
         <is>
           <t>judge</t>
         </is>
-      </c>
-      <c r="I38">
-        <v>8.539999999999999</v>
-      </c>
-      <c r="J38">
-        <v>8.27</v>
       </c>
     </row>
     <row r="39">
@@ -1128,10 +985,7 @@
       <c r="C39">
         <v>6.44</v>
       </c>
-      <c r="F39">
-        <v>6.44</v>
-      </c>
-      <c r="H39" t="inlineStr">
+      <c r="G39" t="inlineStr">
         <is>
           <t>eager</t>
         </is>
@@ -1146,10 +1000,7 @@
       <c r="C40">
         <v>6.44</v>
       </c>
-      <c r="F40">
-        <v>6.44</v>
-      </c>
-      <c r="H40" t="inlineStr">
+      <c r="G40" t="inlineStr">
         <is>
           <t>kiosk</t>
         </is>
@@ -1164,10 +1015,7 @@
       <c r="C41">
         <v>6.44</v>
       </c>
-      <c r="F41">
-        <v>6.44</v>
-      </c>
-      <c r="H41" t="inlineStr">
+      <c r="G41" t="inlineStr">
         <is>
           <t>test</t>
         </is>
@@ -1182,10 +1030,7 @@
       <c r="C42">
         <v>6.45</v>
       </c>
-      <c r="F42">
-        <v>6.45</v>
-      </c>
-      <c r="H42" t="inlineStr">
+      <c r="G42" t="inlineStr">
         <is>
           <t>outer space</t>
         </is>
@@ -1197,16 +1042,13 @@
           <t>geologe</t>
         </is>
       </c>
-      <c r="B43">
+      <c r="C43">
+        <v>6.45</v>
+      </c>
+      <c r="D43">
         <v>1.26</v>
       </c>
-      <c r="D43">
-        <v>6.45</v>
-      </c>
-      <c r="F43">
-        <v>6.45</v>
-      </c>
-      <c r="H43" t="inlineStr">
+      <c r="G43" t="inlineStr">
         <is>
           <t>geologist</t>
         </is>
@@ -1218,16 +1060,13 @@
           <t>steuerberater</t>
         </is>
       </c>
-      <c r="B44">
+      <c r="C44">
+        <v>6.45</v>
+      </c>
+      <c r="D44">
         <v>0.52</v>
       </c>
-      <c r="D44">
-        <v>6.45</v>
-      </c>
-      <c r="F44">
-        <v>6.45</v>
-      </c>
-      <c r="H44" t="inlineStr">
+      <c r="G44" t="inlineStr">
         <is>
           <t>tax advisor</t>
         </is>
@@ -1239,16 +1078,13 @@
           <t>therapeut</t>
         </is>
       </c>
-      <c r="B45">
+      <c r="C45">
+        <v>6.45</v>
+      </c>
+      <c r="D45">
         <v>2.79</v>
       </c>
-      <c r="D45">
-        <v>6.45</v>
-      </c>
-      <c r="F45">
-        <v>6.45</v>
-      </c>
-      <c r="H45" t="inlineStr">
+      <c r="G45" t="inlineStr">
         <is>
           <t>therapist</t>
         </is>
@@ -1263,10 +1099,7 @@
       <c r="C46">
         <v>6.46</v>
       </c>
-      <c r="F46">
-        <v>6.46</v>
-      </c>
-      <c r="H46" t="inlineStr">
+      <c r="G46" t="inlineStr">
         <is>
           <t>popular</t>
         </is>
@@ -1281,10 +1114,7 @@
       <c r="C47">
         <v>6.46</v>
       </c>
-      <c r="F47">
-        <v>6.46</v>
-      </c>
-      <c r="H47" t="inlineStr">
+      <c r="G47" t="inlineStr">
         <is>
           <t>diligence</t>
         </is>
@@ -1299,10 +1129,7 @@
       <c r="C48">
         <v>6.46</v>
       </c>
-      <c r="F48">
-        <v>6.46</v>
-      </c>
-      <c r="H48" t="inlineStr">
+      <c r="G48" t="inlineStr">
         <is>
           <t>food</t>
         </is>
@@ -1317,10 +1144,7 @@
       <c r="C49">
         <v>6.46</v>
       </c>
-      <c r="F49">
-        <v>6.46</v>
-      </c>
-      <c r="H49" t="inlineStr">
+      <c r="G49" t="inlineStr">
         <is>
           <t>ocean</t>
         </is>
@@ -1335,10 +1159,7 @@
       <c r="C50">
         <v>6.46</v>
       </c>
-      <c r="F50">
-        <v>6.46</v>
-      </c>
-      <c r="H50" t="inlineStr">
+      <c r="G50" t="inlineStr">
         <is>
           <t>spook</t>
         </is>
@@ -1353,10 +1174,7 @@
       <c r="C51">
         <v>6.47</v>
       </c>
-      <c r="F51">
-        <v>6.47</v>
-      </c>
-      <c r="H51" t="inlineStr">
+      <c r="G51" t="inlineStr">
         <is>
           <t>take up</t>
         </is>
@@ -1371,10 +1189,7 @@
       <c r="C52">
         <v>6.47</v>
       </c>
-      <c r="F52">
-        <v>6.47</v>
-      </c>
-      <c r="H52" t="inlineStr">
+      <c r="G52" t="inlineStr">
         <is>
           <t>require</t>
         </is>
@@ -1389,10 +1204,7 @@
       <c r="C53">
         <v>6.47</v>
       </c>
-      <c r="F53">
-        <v>6.47</v>
-      </c>
-      <c r="H53" t="inlineStr">
+      <c r="G53" t="inlineStr">
         <is>
           <t>mastiff</t>
         </is>
@@ -1407,10 +1219,7 @@
       <c r="C54">
         <v>6.47</v>
       </c>
-      <c r="F54">
-        <v>6.47</v>
-      </c>
-      <c r="H54" t="inlineStr">
+      <c r="G54" t="inlineStr">
         <is>
           <t>advantage</t>
         </is>
@@ -1422,16 +1231,13 @@
           <t>fräser</t>
         </is>
       </c>
-      <c r="B55">
+      <c r="C55">
+        <v>6.47</v>
+      </c>
+      <c r="D55">
         <v>0.07000000000000001</v>
       </c>
-      <c r="D55">
-        <v>6.47</v>
-      </c>
-      <c r="F55">
-        <v>6.47</v>
-      </c>
-      <c r="H55" t="inlineStr">
+      <c r="G55" t="inlineStr">
         <is>
           <t>milling cutter</t>
         </is>
@@ -1446,10 +1252,7 @@
       <c r="C56">
         <v>6.48</v>
       </c>
-      <c r="F56">
-        <v>6.48</v>
-      </c>
-      <c r="H56" t="inlineStr">
+      <c r="G56" t="inlineStr">
         <is>
           <t>envy</t>
         </is>
@@ -1464,10 +1267,7 @@
       <c r="C57">
         <v>6.48</v>
       </c>
-      <c r="F57">
-        <v>6.48</v>
-      </c>
-      <c r="H57" t="inlineStr">
+      <c r="G57" t="inlineStr">
         <is>
           <t>duty</t>
         </is>
@@ -1482,10 +1282,7 @@
       <c r="C58">
         <v>6.48</v>
       </c>
-      <c r="F58">
-        <v>6.48</v>
-      </c>
-      <c r="H58" t="inlineStr">
+      <c r="G58" t="inlineStr">
         <is>
           <t>glen</t>
         </is>
@@ -1500,10 +1297,7 @@
       <c r="C59">
         <v>6.5</v>
       </c>
-      <c r="F59">
-        <v>6.5</v>
-      </c>
-      <c r="H59" t="inlineStr">
+      <c r="G59" t="inlineStr">
         <is>
           <t>respect</t>
         </is>
@@ -1518,10 +1312,7 @@
       <c r="C60">
         <v>6.5</v>
       </c>
-      <c r="F60">
-        <v>6.5</v>
-      </c>
-      <c r="H60" t="inlineStr">
+      <c r="G60" t="inlineStr">
         <is>
           <t>outburst</t>
         </is>
@@ -1536,10 +1327,7 @@
       <c r="C61">
         <v>6.5</v>
       </c>
-      <c r="F61">
-        <v>6.5</v>
-      </c>
-      <c r="H61" t="inlineStr">
+      <c r="G61" t="inlineStr">
         <is>
           <t>mean</t>
         </is>
@@ -1554,10 +1342,7 @@
       <c r="C62">
         <v>6.5</v>
       </c>
-      <c r="F62">
-        <v>6.5</v>
-      </c>
-      <c r="H62" t="inlineStr">
+      <c r="G62" t="inlineStr">
         <is>
           <t>improvement</t>
         </is>
@@ -1572,10 +1357,7 @@
       <c r="C63">
         <v>6.5</v>
       </c>
-      <c r="F63">
-        <v>6.5</v>
-      </c>
-      <c r="H63" t="inlineStr">
+      <c r="G63" t="inlineStr">
         <is>
           <t>happen</t>
         </is>
@@ -1590,10 +1372,7 @@
       <c r="C64">
         <v>6.5</v>
       </c>
-      <c r="F64">
-        <v>6.5</v>
-      </c>
-      <c r="H64" t="inlineStr">
+      <c r="G64" t="inlineStr">
         <is>
           <t>catch</t>
         </is>
@@ -1608,10 +1387,7 @@
       <c r="C65">
         <v>6.5</v>
       </c>
-      <c r="F65">
-        <v>6.5</v>
-      </c>
-      <c r="H65" t="inlineStr">
+      <c r="G65" t="inlineStr">
         <is>
           <t>frosty</t>
         </is>
@@ -1626,10 +1402,7 @@
       <c r="C66">
         <v>6.5</v>
       </c>
-      <c r="F66">
-        <v>6.5</v>
-      </c>
-      <c r="H66" t="inlineStr">
+      <c r="G66" t="inlineStr">
         <is>
           <t>curing</t>
         </is>
@@ -1644,10 +1417,7 @@
       <c r="C67">
         <v>6.5</v>
       </c>
-      <c r="F67">
-        <v>6.5</v>
-      </c>
-      <c r="H67" t="inlineStr">
+      <c r="G67" t="inlineStr">
         <is>
           <t>perfect</t>
         </is>
@@ -1662,10 +1432,7 @@
       <c r="C68">
         <v>6.5</v>
       </c>
-      <c r="F68">
-        <v>6.5</v>
-      </c>
-      <c r="H68" t="inlineStr">
+      <c r="G68" t="inlineStr">
         <is>
           <t>imagine</t>
         </is>
@@ -1677,16 +1444,13 @@
           <t>litschi</t>
         </is>
       </c>
-      <c r="B69">
+      <c r="C69">
+        <v>6.5</v>
+      </c>
+      <c r="D69">
         <v>0.03</v>
       </c>
-      <c r="D69">
-        <v>6.5</v>
-      </c>
-      <c r="F69">
-        <v>6.5</v>
-      </c>
-      <c r="H69" t="inlineStr">
+      <c r="G69" t="inlineStr">
         <is>
           <t>lychee</t>
         </is>
@@ -1698,16 +1462,13 @@
           <t>papaya</t>
         </is>
       </c>
-      <c r="B70">
+      <c r="C70">
+        <v>6.5</v>
+      </c>
+      <c r="D70">
         <v>0.1</v>
       </c>
-      <c r="D70">
-        <v>6.5</v>
-      </c>
-      <c r="F70">
-        <v>6.5</v>
-      </c>
-      <c r="H70" t="inlineStr">
+      <c r="G70" t="inlineStr">
         <is>
           <t>papaya</t>
         </is>
@@ -1719,16 +1480,13 @@
           <t>draisine</t>
         </is>
       </c>
-      <c r="B71">
+      <c r="C71">
+        <v>6.5</v>
+      </c>
+      <c r="D71">
         <v>0.13</v>
       </c>
-      <c r="D71">
-        <v>6.5</v>
-      </c>
-      <c r="F71">
-        <v>6.5</v>
-      </c>
-      <c r="H71" t="inlineStr">
+      <c r="G71" t="inlineStr">
         <is>
           <t>rail trolley</t>
         </is>
@@ -1740,16 +1498,13 @@
           <t>breakdance</t>
         </is>
       </c>
-      <c r="B72">
+      <c r="C72">
+        <v>6.5</v>
+      </c>
+      <c r="D72">
         <v>0.01</v>
       </c>
-      <c r="D72">
-        <v>6.5</v>
-      </c>
-      <c r="F72">
-        <v>6.5</v>
-      </c>
-      <c r="H72" t="inlineStr">
+      <c r="G72" t="inlineStr">
         <is>
           <t>break dancing</t>
         </is>
@@ -1761,16 +1516,13 @@
           <t>cricket</t>
         </is>
       </c>
-      <c r="B73">
+      <c r="C73">
+        <v>6.5</v>
+      </c>
+      <c r="D73">
         <v>0.03</v>
       </c>
-      <c r="D73">
-        <v>6.5</v>
-      </c>
-      <c r="F73">
-        <v>6.5</v>
-      </c>
-      <c r="H73" t="inlineStr">
+      <c r="G73" t="inlineStr">
         <is>
           <t>cricket</t>
         </is>
@@ -1782,13 +1534,10 @@
           <t>drachenbootrennen</t>
         </is>
       </c>
-      <c r="D74">
+      <c r="C74">
         <v>6.5</v>
       </c>
-      <c r="F74">
-        <v>6.5</v>
-      </c>
-      <c r="H74" t="inlineStr">
+      <c r="G74" t="inlineStr">
         <is>
           <t>dragon boat racing</t>
         </is>
@@ -1800,16 +1549,13 @@
           <t>psychotherapeut</t>
         </is>
       </c>
-      <c r="B75">
+      <c r="C75">
+        <v>6.5</v>
+      </c>
+      <c r="D75">
         <v>0.6899999999999999</v>
       </c>
-      <c r="D75">
-        <v>6.5</v>
-      </c>
-      <c r="F75">
-        <v>6.5</v>
-      </c>
-      <c r="H75" t="inlineStr">
+      <c r="G75" t="inlineStr">
         <is>
           <t>psychotherapist</t>
         </is>
@@ -1824,10 +1570,7 @@
       <c r="C76">
         <v>6.52</v>
       </c>
-      <c r="F76">
-        <v>6.52</v>
-      </c>
-      <c r="H76" t="inlineStr">
+      <c r="G76" t="inlineStr">
         <is>
           <t>earthquake</t>
         </is>
@@ -1842,10 +1585,7 @@
       <c r="C77">
         <v>6.52</v>
       </c>
-      <c r="F77">
-        <v>6.52</v>
-      </c>
-      <c r="H77" t="inlineStr">
+      <c r="G77" t="inlineStr">
         <is>
           <t>obtain</t>
         </is>
@@ -1860,10 +1600,7 @@
       <c r="C78">
         <v>6.52</v>
       </c>
-      <c r="F78">
-        <v>6.52</v>
-      </c>
-      <c r="H78" t="inlineStr">
+      <c r="G78" t="inlineStr">
         <is>
           <t>centimetre</t>
         </is>
@@ -1875,13 +1612,10 @@
           <t>heißluftpistole</t>
         </is>
       </c>
-      <c r="D79">
+      <c r="C79">
         <v>6.53</v>
       </c>
-      <c r="F79">
-        <v>6.53</v>
-      </c>
-      <c r="H79" t="inlineStr">
+      <c r="G79" t="inlineStr">
         <is>
           <t>hot air gun</t>
         </is>
@@ -1896,10 +1630,7 @@
       <c r="C80">
         <v>6.53</v>
       </c>
-      <c r="F80">
-        <v>6.53</v>
-      </c>
-      <c r="H80" t="inlineStr">
+      <c r="G80" t="inlineStr">
         <is>
           <t>ankle</t>
         </is>
@@ -1911,19 +1642,13 @@
           <t>kobra</t>
         </is>
       </c>
-      <c r="B81">
-        <v>0.33</v>
-      </c>
       <c r="C81">
         <v>6.53</v>
       </c>
       <c r="D81">
-        <v>4</v>
-      </c>
-      <c r="F81">
-        <v>6.53</v>
-      </c>
-      <c r="H81" t="inlineStr">
+        <v>0.33</v>
+      </c>
+      <c r="G81" t="inlineStr">
         <is>
           <t>cobra</t>
         </is>
@@ -1938,10 +1663,7 @@
       <c r="C82">
         <v>6.53</v>
       </c>
-      <c r="F82">
-        <v>6.53</v>
-      </c>
-      <c r="H82" t="inlineStr">
+      <c r="G82" t="inlineStr">
         <is>
           <t>comma</t>
         </is>
@@ -1956,10 +1678,7 @@
       <c r="C83">
         <v>6.53</v>
       </c>
-      <c r="F83">
-        <v>6.53</v>
-      </c>
-      <c r="H83" t="inlineStr">
+      <c r="G83" t="inlineStr">
         <is>
           <t>cargo</t>
         </is>
@@ -1974,10 +1693,7 @@
       <c r="C84">
         <v>6.53</v>
       </c>
-      <c r="F84">
-        <v>6.53</v>
-      </c>
-      <c r="H84" t="inlineStr">
+      <c r="G84" t="inlineStr">
         <is>
           <t>oily</t>
         </is>
@@ -1992,10 +1708,7 @@
       <c r="C85">
         <v>6.53</v>
       </c>
-      <c r="F85">
-        <v>6.53</v>
-      </c>
-      <c r="H85" t="inlineStr">
+      <c r="G85" t="inlineStr">
         <is>
           <t>grieve</t>
         </is>
@@ -2010,10 +1723,7 @@
       <c r="C86">
         <v>6.53</v>
       </c>
-      <c r="F86">
-        <v>6.53</v>
-      </c>
-      <c r="H86" t="inlineStr">
+      <c r="G86" t="inlineStr">
         <is>
           <t>tackle</t>
         </is>
@@ -2025,16 +1735,13 @@
           <t>pharmareferent</t>
         </is>
       </c>
-      <c r="B87">
+      <c r="C87">
+        <v>6.53</v>
+      </c>
+      <c r="D87">
         <v>0.01</v>
       </c>
-      <c r="D87">
-        <v>6.53</v>
-      </c>
-      <c r="F87">
-        <v>6.53</v>
-      </c>
-      <c r="H87" t="inlineStr">
+      <c r="G87" t="inlineStr">
         <is>
           <t>medical representative</t>
         </is>
@@ -2049,10 +1756,7 @@
       <c r="C88">
         <v>6.54</v>
       </c>
-      <c r="F88">
-        <v>6.54</v>
-      </c>
-      <c r="H88" t="inlineStr">
+      <c r="G88" t="inlineStr">
         <is>
           <t>inventor</t>
         </is>
@@ -2067,10 +1771,7 @@
       <c r="C89">
         <v>6.54</v>
       </c>
-      <c r="F89">
-        <v>6.54</v>
-      </c>
-      <c r="H89" t="inlineStr">
+      <c r="G89" t="inlineStr">
         <is>
           <t>marvellous</t>
         </is>
@@ -2085,10 +1786,7 @@
       <c r="C90">
         <v>6.54</v>
       </c>
-      <c r="F90">
-        <v>6.54</v>
-      </c>
-      <c r="H90" t="inlineStr">
+      <c r="G90" t="inlineStr">
         <is>
           <t>produce</t>
         </is>
@@ -2103,10 +1801,7 @@
       <c r="C91">
         <v>6.54</v>
       </c>
-      <c r="F91">
-        <v>6.54</v>
-      </c>
-      <c r="H91" t="inlineStr">
+      <c r="G91" t="inlineStr">
         <is>
           <t>opinion</t>
         </is>
@@ -2121,10 +1816,7 @@
       <c r="C92">
         <v>6.54</v>
       </c>
-      <c r="F92">
-        <v>6.54</v>
-      </c>
-      <c r="H92" t="inlineStr">
+      <c r="G92" t="inlineStr">
         <is>
           <t>will</t>
         </is>
@@ -2139,10 +1831,7 @@
       <c r="C93">
         <v>6.55</v>
       </c>
-      <c r="F93">
-        <v>6.55</v>
-      </c>
-      <c r="H93" t="inlineStr">
+      <c r="G93" t="inlineStr">
         <is>
           <t>know-all</t>
         </is>
@@ -2154,13 +1843,10 @@
           <t>streetdance</t>
         </is>
       </c>
-      <c r="D94">
+      <c r="C94">
         <v>6.55</v>
       </c>
-      <c r="F94">
-        <v>6.55</v>
-      </c>
-      <c r="H94" t="inlineStr">
+      <c r="G94" t="inlineStr">
         <is>
           <t>street dance</t>
         </is>
@@ -2172,16 +1858,13 @@
           <t>informatiker</t>
         </is>
       </c>
-      <c r="B95">
+      <c r="C95">
+        <v>6.55</v>
+      </c>
+      <c r="D95">
         <v>0.63</v>
       </c>
-      <c r="D95">
-        <v>6.55</v>
-      </c>
-      <c r="F95">
-        <v>6.55</v>
-      </c>
-      <c r="H95" t="inlineStr">
+      <c r="G95" t="inlineStr">
         <is>
           <t>computer scientist</t>
         </is>
@@ -2193,16 +1876,13 @@
           <t>grafikdesigner</t>
         </is>
       </c>
-      <c r="B96">
+      <c r="C96">
+        <v>6.55</v>
+      </c>
+      <c r="D96">
         <v>0.02</v>
       </c>
-      <c r="D96">
-        <v>6.55</v>
-      </c>
-      <c r="F96">
-        <v>6.55</v>
-      </c>
-      <c r="H96" t="inlineStr">
+      <c r="G96" t="inlineStr">
         <is>
           <t>graphic designer</t>
         </is>
@@ -2214,16 +1894,13 @@
           <t>gynäkologe</t>
         </is>
       </c>
-      <c r="B97">
+      <c r="C97">
+        <v>6.55</v>
+      </c>
+      <c r="D97">
         <v>0.6</v>
       </c>
-      <c r="D97">
-        <v>6.55</v>
-      </c>
-      <c r="F97">
-        <v>6.55</v>
-      </c>
-      <c r="H97" t="inlineStr">
+      <c r="G97" t="inlineStr">
         <is>
           <t>gynaecologist</t>
         </is>
@@ -2235,13 +1912,10 @@
           <t>logopäde</t>
         </is>
       </c>
-      <c r="D98">
+      <c r="C98">
         <v>6.55</v>
       </c>
-      <c r="F98">
-        <v>6.55</v>
-      </c>
-      <c r="H98" t="inlineStr">
+      <c r="G98" t="inlineStr">
         <is>
           <t>speech therapist</t>
         </is>
@@ -2256,10 +1930,7 @@
       <c r="C99">
         <v>6.56</v>
       </c>
-      <c r="F99">
-        <v>6.56</v>
-      </c>
-      <c r="H99" t="inlineStr">
+      <c r="G99" t="inlineStr">
         <is>
           <t>company</t>
         </is>
@@ -2274,10 +1945,7 @@
       <c r="C100">
         <v>6.56</v>
       </c>
-      <c r="F100">
-        <v>6.56</v>
-      </c>
-      <c r="H100" t="inlineStr">
+      <c r="G100" t="inlineStr">
         <is>
           <t>message</t>
         </is>
@@ -2292,10 +1960,7 @@
       <c r="C101">
         <v>6.56</v>
       </c>
-      <c r="F101">
-        <v>6.56</v>
-      </c>
-      <c r="H101" t="inlineStr">
+      <c r="G101" t="inlineStr">
         <is>
           <t>perfume</t>
         </is>
@@ -2310,10 +1975,7 @@
       <c r="C102">
         <v>6.56</v>
       </c>
-      <c r="F102">
-        <v>6.56</v>
-      </c>
-      <c r="H102" t="inlineStr">
+      <c r="G102" t="inlineStr">
         <is>
           <t>will</t>
         </is>
@@ -2328,10 +1990,7 @@
       <c r="C103">
         <v>6.57</v>
       </c>
-      <c r="F103">
-        <v>6.57</v>
-      </c>
-      <c r="H103" t="inlineStr">
+      <c r="G103" t="inlineStr">
         <is>
           <t>moth</t>
         </is>
@@ -2346,10 +2005,7 @@
       <c r="C104">
         <v>6.57</v>
       </c>
-      <c r="F104">
-        <v>6.57</v>
-      </c>
-      <c r="H104" t="inlineStr">
+      <c r="G104" t="inlineStr">
         <is>
           <t>palm tree</t>
         </is>
@@ -2364,10 +2020,7 @@
       <c r="C105">
         <v>6.57</v>
       </c>
-      <c r="F105">
-        <v>6.57</v>
-      </c>
-      <c r="H105" t="inlineStr">
+      <c r="G105" t="inlineStr">
         <is>
           <t>sway</t>
         </is>
@@ -2382,10 +2035,7 @@
       <c r="C106">
         <v>6.57</v>
       </c>
-      <c r="F106">
-        <v>6.57</v>
-      </c>
-      <c r="H106" t="inlineStr">
+      <c r="G106" t="inlineStr">
         <is>
           <t>sinking</t>
         </is>
@@ -2400,10 +2050,7 @@
       <c r="C107">
         <v>6.57</v>
       </c>
-      <c r="F107">
-        <v>6.57</v>
-      </c>
-      <c r="H107" t="inlineStr">
+      <c r="G107" t="inlineStr">
         <is>
           <t>have an effect</t>
         </is>
@@ -2415,16 +2062,13 @@
           <t>paragleiten</t>
         </is>
       </c>
-      <c r="B108">
+      <c r="C108">
+        <v>6.58</v>
+      </c>
+      <c r="D108">
         <v>0.01</v>
       </c>
-      <c r="D108">
-        <v>6.58</v>
-      </c>
-      <c r="F108">
-        <v>6.58</v>
-      </c>
-      <c r="H108" t="inlineStr">
+      <c r="G108" t="inlineStr">
         <is>
           <t>paragliding</t>
         </is>
@@ -2436,16 +2080,13 @@
           <t>gerichtsvollzieher</t>
         </is>
       </c>
-      <c r="B109">
+      <c r="C109">
+        <v>6.58</v>
+      </c>
+      <c r="D109">
         <v>2.2</v>
       </c>
-      <c r="D109">
-        <v>6.58</v>
-      </c>
-      <c r="F109">
-        <v>6.58</v>
-      </c>
-      <c r="H109" t="inlineStr">
+      <c r="G109" t="inlineStr">
         <is>
           <t>bailiff</t>
         </is>
@@ -2460,10 +2101,7 @@
       <c r="C110">
         <v>6.58</v>
       </c>
-      <c r="F110">
-        <v>6.58</v>
-      </c>
-      <c r="H110" t="inlineStr">
+      <c r="G110" t="inlineStr">
         <is>
           <t>reject</t>
         </is>
@@ -2478,10 +2116,7 @@
       <c r="C111">
         <v>6.58</v>
       </c>
-      <c r="F111">
-        <v>6.58</v>
-      </c>
-      <c r="H111" t="inlineStr">
+      <c r="G111" t="inlineStr">
         <is>
           <t>clarify</t>
         </is>
@@ -2496,10 +2131,7 @@
       <c r="C112">
         <v>6.58</v>
       </c>
-      <c r="F112">
-        <v>6.58</v>
-      </c>
-      <c r="H112" t="inlineStr">
+      <c r="G112" t="inlineStr">
         <is>
           <t>cleverness</t>
         </is>
@@ -2514,10 +2146,7 @@
       <c r="C113">
         <v>6.58</v>
       </c>
-      <c r="F113">
-        <v>6.58</v>
-      </c>
-      <c r="H113" t="inlineStr">
+      <c r="G113" t="inlineStr">
         <is>
           <t>list</t>
         </is>
@@ -2532,10 +2161,7 @@
       <c r="C114">
         <v>6.58</v>
       </c>
-      <c r="F114">
-        <v>6.58</v>
-      </c>
-      <c r="H114" t="inlineStr">
+      <c r="G114" t="inlineStr">
         <is>
           <t>magical</t>
         </is>
@@ -2550,10 +2176,7 @@
       <c r="C115">
         <v>6.59</v>
       </c>
-      <c r="F115">
-        <v>6.59</v>
-      </c>
-      <c r="H115" t="inlineStr">
+      <c r="G115" t="inlineStr">
         <is>
           <t>worried</t>
         </is>
@@ -2568,10 +2191,7 @@
       <c r="C116">
         <v>6.59</v>
       </c>
-      <c r="F116">
-        <v>6.59</v>
-      </c>
-      <c r="H116" t="inlineStr">
+      <c r="G116" t="inlineStr">
         <is>
           <t>only</t>
         </is>
@@ -2586,10 +2206,7 @@
       <c r="C117">
         <v>6.59</v>
       </c>
-      <c r="F117">
-        <v>6.59</v>
-      </c>
-      <c r="H117" t="inlineStr">
+      <c r="G117" t="inlineStr">
         <is>
           <t>expect</t>
         </is>
@@ -2604,10 +2221,7 @@
       <c r="C118">
         <v>6.59</v>
       </c>
-      <c r="F118">
-        <v>6.59</v>
-      </c>
-      <c r="H118" t="inlineStr">
+      <c r="G118" t="inlineStr">
         <is>
           <t>muscle</t>
         </is>
@@ -2622,10 +2236,7 @@
       <c r="C119">
         <v>6.59</v>
       </c>
-      <c r="F119">
-        <v>6.59</v>
-      </c>
-      <c r="H119" t="inlineStr">
+      <c r="G119" t="inlineStr">
         <is>
           <t>goblet</t>
         </is>
@@ -2640,10 +2251,7 @@
       <c r="C120">
         <v>6.59</v>
       </c>
-      <c r="F120">
-        <v>6.59</v>
-      </c>
-      <c r="H120" t="inlineStr">
+      <c r="G120" t="inlineStr">
         <is>
           <t>stare</t>
         </is>
@@ -2658,10 +2266,7 @@
       <c r="C121">
         <v>6.59</v>
       </c>
-      <c r="F121">
-        <v>6.59</v>
-      </c>
-      <c r="H121" t="inlineStr">
+      <c r="G121" t="inlineStr">
         <is>
           <t>ventilator</t>
         </is>
@@ -2676,10 +2281,7 @@
       <c r="C122">
         <v>6.6</v>
       </c>
-      <c r="F122">
-        <v>6.6</v>
-      </c>
-      <c r="H122" t="inlineStr">
+      <c r="G122" t="inlineStr">
         <is>
           <t>grab</t>
         </is>
@@ -2694,10 +2296,7 @@
       <c r="C123">
         <v>6.6</v>
       </c>
-      <c r="F123">
-        <v>6.6</v>
-      </c>
-      <c r="H123" t="inlineStr">
+      <c r="G123" t="inlineStr">
         <is>
           <t>scorpion</t>
         </is>
@@ -2709,16 +2308,13 @@
           <t>lektor</t>
         </is>
       </c>
-      <c r="B124">
+      <c r="C124">
+        <v>6.6</v>
+      </c>
+      <c r="D124">
         <v>2.46</v>
       </c>
-      <c r="D124">
-        <v>6.6</v>
-      </c>
-      <c r="F124">
-        <v>6.6</v>
-      </c>
-      <c r="H124" t="inlineStr">
+      <c r="G124" t="inlineStr">
         <is>
           <t>lecturer</t>
         </is>
@@ -2730,16 +2326,13 @@
           <t>unternehmensberater</t>
         </is>
       </c>
-      <c r="B125">
+      <c r="C125">
+        <v>6.6</v>
+      </c>
+      <c r="D125">
         <v>0.18</v>
       </c>
-      <c r="D125">
-        <v>6.6</v>
-      </c>
-      <c r="F125">
-        <v>6.6</v>
-      </c>
-      <c r="H125" t="inlineStr">
+      <c r="G125" t="inlineStr">
         <is>
           <t>management consultant</t>
         </is>
@@ -2751,16 +2344,13 @@
           <t>pathologe</t>
         </is>
       </c>
-      <c r="B126">
+      <c r="C126">
+        <v>6.6</v>
+      </c>
+      <c r="D126">
         <v>0.2</v>
       </c>
-      <c r="D126">
-        <v>6.6</v>
-      </c>
-      <c r="F126">
-        <v>6.6</v>
-      </c>
-      <c r="H126" t="inlineStr">
+      <c r="G126" t="inlineStr">
         <is>
           <t>pathologist</t>
         </is>
@@ -2775,10 +2365,7 @@
       <c r="C127">
         <v>6.61</v>
       </c>
-      <c r="F127">
-        <v>6.61</v>
-      </c>
-      <c r="H127" t="inlineStr">
+      <c r="G127" t="inlineStr">
         <is>
           <t>assume</t>
         </is>
@@ -2790,19 +2377,13 @@
           <t>fasan</t>
         </is>
       </c>
-      <c r="B128">
-        <v>1.5</v>
-      </c>
       <c r="C128">
         <v>6.61</v>
       </c>
       <c r="D128">
-        <v>4.65</v>
-      </c>
-      <c r="F128">
-        <v>6.61</v>
-      </c>
-      <c r="H128" t="inlineStr">
+        <v>1.5</v>
+      </c>
+      <c r="G128" t="inlineStr">
         <is>
           <t>pheasant</t>
         </is>
@@ -2817,10 +2398,7 @@
       <c r="C129">
         <v>6.61</v>
       </c>
-      <c r="F129">
-        <v>6.61</v>
-      </c>
-      <c r="H129" t="inlineStr">
+      <c r="G129" t="inlineStr">
         <is>
           <t>helpless</t>
         </is>
@@ -2835,10 +2413,7 @@
       <c r="C130">
         <v>6.61</v>
       </c>
-      <c r="F130">
-        <v>6.61</v>
-      </c>
-      <c r="H130" t="inlineStr">
+      <c r="G130" t="inlineStr">
         <is>
           <t>scenery</t>
         </is>
@@ -2853,10 +2428,7 @@
       <c r="C131">
         <v>6.61</v>
       </c>
-      <c r="F131">
-        <v>6.61</v>
-      </c>
-      <c r="H131" t="inlineStr">
+      <c r="G131" t="inlineStr">
         <is>
           <t>party</t>
         </is>
@@ -2871,10 +2443,7 @@
       <c r="C132">
         <v>6.62</v>
       </c>
-      <c r="F132">
-        <v>6.62</v>
-      </c>
-      <c r="H132" t="inlineStr">
+      <c r="G132" t="inlineStr">
         <is>
           <t>rule</t>
         </is>
@@ -2889,10 +2458,7 @@
       <c r="C133">
         <v>6.63</v>
       </c>
-      <c r="F133">
-        <v>6.63</v>
-      </c>
-      <c r="H133" t="inlineStr">
+      <c r="G133" t="inlineStr">
         <is>
           <t>alphabetic</t>
         </is>
@@ -2907,10 +2473,7 @@
       <c r="C134">
         <v>6.63</v>
       </c>
-      <c r="F134">
-        <v>6.63</v>
-      </c>
-      <c r="H134" t="inlineStr">
+      <c r="G134" t="inlineStr">
         <is>
           <t>mythical creature</t>
         </is>
@@ -2925,10 +2488,7 @@
       <c r="C135">
         <v>6.63</v>
       </c>
-      <c r="F135">
-        <v>6.63</v>
-      </c>
-      <c r="H135" t="inlineStr">
+      <c r="G135" t="inlineStr">
         <is>
           <t>freedom</t>
         </is>
@@ -2943,10 +2503,7 @@
       <c r="C136">
         <v>6.63</v>
       </c>
-      <c r="F136">
-        <v>6.63</v>
-      </c>
-      <c r="H136" t="inlineStr">
+      <c r="G136" t="inlineStr">
         <is>
           <t>reign</t>
         </is>
@@ -2961,10 +2518,7 @@
       <c r="C137">
         <v>6.63</v>
       </c>
-      <c r="F137">
-        <v>6.63</v>
-      </c>
-      <c r="H137" t="inlineStr">
+      <c r="G137" t="inlineStr">
         <is>
           <t>hearty</t>
         </is>
@@ -2979,10 +2533,7 @@
       <c r="C138">
         <v>6.63</v>
       </c>
-      <c r="F138">
-        <v>6.63</v>
-      </c>
-      <c r="H138" t="inlineStr">
+      <c r="G138" t="inlineStr">
         <is>
           <t>labyrinth</t>
         </is>
@@ -2997,10 +2548,7 @@
       <c r="C139">
         <v>6.63</v>
       </c>
-      <c r="F139">
-        <v>6.63</v>
-      </c>
-      <c r="H139" t="inlineStr">
+      <c r="G139" t="inlineStr">
         <is>
           <t>painting</t>
         </is>
@@ -3015,10 +2563,7 @@
       <c r="C140">
         <v>6.63</v>
       </c>
-      <c r="F140">
-        <v>6.63</v>
-      </c>
-      <c r="H140" t="inlineStr">
+      <c r="G140" t="inlineStr">
         <is>
           <t>oil</t>
         </is>
@@ -3033,10 +2578,7 @@
       <c r="C141">
         <v>6.63</v>
       </c>
-      <c r="F141">
-        <v>6.63</v>
-      </c>
-      <c r="H141" t="inlineStr">
+      <c r="G141" t="inlineStr">
         <is>
           <t>joke</t>
         </is>
@@ -3051,10 +2593,7 @@
       <c r="C142">
         <v>6.63</v>
       </c>
-      <c r="F142">
-        <v>6.63</v>
-      </c>
-      <c r="H142" t="inlineStr">
+      <c r="G142" t="inlineStr">
         <is>
           <t>stiff</t>
         </is>
@@ -3069,10 +2608,7 @@
       <c r="C143">
         <v>6.63</v>
       </c>
-      <c r="F143">
-        <v>6.63</v>
-      </c>
-      <c r="H143" t="inlineStr">
+      <c r="G143" t="inlineStr">
         <is>
           <t>tobacco</t>
         </is>
@@ -3087,10 +2623,7 @@
       <c r="C144">
         <v>6.63</v>
       </c>
-      <c r="F144">
-        <v>6.63</v>
-      </c>
-      <c r="H144" t="inlineStr">
+      <c r="G144" t="inlineStr">
         <is>
           <t>title</t>
         </is>
@@ -3102,16 +2635,13 @@
           <t>gerichtshilfe</t>
         </is>
       </c>
-      <c r="B145">
+      <c r="C145">
+        <v>6.63</v>
+      </c>
+      <c r="D145">
         <v>0.16</v>
       </c>
-      <c r="D145">
-        <v>6.63</v>
-      </c>
-      <c r="F145">
-        <v>6.63</v>
-      </c>
-      <c r="H145" t="inlineStr">
+      <c r="G145" t="inlineStr">
         <is>
           <t>court assistant</t>
         </is>
@@ -3123,16 +2653,13 @@
           <t>dramaturg</t>
         </is>
       </c>
-      <c r="B146">
+      <c r="C146">
+        <v>6.63</v>
+      </c>
+      <c r="D146">
         <v>1.23</v>
       </c>
-      <c r="D146">
-        <v>6.63</v>
-      </c>
-      <c r="F146">
-        <v>6.63</v>
-      </c>
-      <c r="H146" t="inlineStr">
+      <c r="G146" t="inlineStr">
         <is>
           <t>playwright</t>
         </is>
@@ -3147,10 +2674,7 @@
       <c r="C147">
         <v>6.64</v>
       </c>
-      <c r="F147">
-        <v>6.64</v>
-      </c>
-      <c r="H147" t="inlineStr">
+      <c r="G147" t="inlineStr">
         <is>
           <t>atlas</t>
         </is>
@@ -3165,10 +2689,7 @@
       <c r="C148">
         <v>6.64</v>
       </c>
-      <c r="F148">
-        <v>6.64</v>
-      </c>
-      <c r="H148" t="inlineStr">
+      <c r="G148" t="inlineStr">
         <is>
           <t>chaos</t>
         </is>
@@ -3183,10 +2704,7 @@
       <c r="C149">
         <v>6.64</v>
       </c>
-      <c r="F149">
-        <v>6.64</v>
-      </c>
-      <c r="H149" t="inlineStr">
+      <c r="G149" t="inlineStr">
         <is>
           <t>problem</t>
         </is>
@@ -3201,10 +2719,7 @@
       <c r="C150">
         <v>6.64</v>
       </c>
-      <c r="F150">
-        <v>6.64</v>
-      </c>
-      <c r="H150" t="inlineStr">
+      <c r="G150" t="inlineStr">
         <is>
           <t>consideration</t>
         </is>
@@ -3219,10 +2734,7 @@
       <c r="C151">
         <v>6.64</v>
       </c>
-      <c r="F151">
-        <v>6.64</v>
-      </c>
-      <c r="H151" t="inlineStr">
+      <c r="G151" t="inlineStr">
         <is>
           <t>hover</t>
         </is>
@@ -3237,10 +2749,7 @@
       <c r="C152">
         <v>6.65</v>
       </c>
-      <c r="F152">
-        <v>6.65</v>
-      </c>
-      <c r="H152" t="inlineStr">
+      <c r="G152" t="inlineStr">
         <is>
           <t>glaze</t>
         </is>
@@ -3255,10 +2764,7 @@
       <c r="C153">
         <v>6.65</v>
       </c>
-      <c r="F153">
-        <v>6.65</v>
-      </c>
-      <c r="H153" t="inlineStr">
+      <c r="G153" t="inlineStr">
         <is>
           <t>tease</t>
         </is>
@@ -3273,10 +2779,7 @@
       <c r="C154">
         <v>6.65</v>
       </c>
-      <c r="F154">
-        <v>6.65</v>
-      </c>
-      <c r="H154" t="inlineStr">
+      <c r="G154" t="inlineStr">
         <is>
           <t>wagon</t>
         </is>
@@ -3288,13 +2791,10 @@
           <t>mediendesigner</t>
         </is>
       </c>
-      <c r="D155">
+      <c r="C155">
         <v>6.65</v>
       </c>
-      <c r="F155">
-        <v>6.65</v>
-      </c>
-      <c r="H155" t="inlineStr">
+      <c r="G155" t="inlineStr">
         <is>
           <t>media designer</t>
         </is>
@@ -3306,16 +2806,13 @@
           <t>sozialpädagoge</t>
         </is>
       </c>
-      <c r="B156">
+      <c r="C156">
+        <v>6.65</v>
+      </c>
+      <c r="D156">
         <v>0.19</v>
       </c>
-      <c r="D156">
-        <v>6.65</v>
-      </c>
-      <c r="F156">
-        <v>6.65</v>
-      </c>
-      <c r="H156" t="inlineStr">
+      <c r="G156" t="inlineStr">
         <is>
           <t>social worker</t>
         </is>
@@ -3327,13 +2824,10 @@
           <t>sportassistent</t>
         </is>
       </c>
-      <c r="D157">
+      <c r="C157">
         <v>6.65</v>
       </c>
-      <c r="F157">
-        <v>6.65</v>
-      </c>
-      <c r="H157" t="inlineStr">
+      <c r="G157" t="inlineStr">
         <is>
           <t>sports assistant</t>
         </is>
@@ -3345,13 +2839,10 @@
           <t>sporttherapeut</t>
         </is>
       </c>
-      <c r="D158">
+      <c r="C158">
         <v>6.65</v>
       </c>
-      <c r="F158">
-        <v>6.65</v>
-      </c>
-      <c r="H158" t="inlineStr">
+      <c r="G158" t="inlineStr">
         <is>
           <t>sports therapist</t>
         </is>
@@ -3363,16 +2854,13 @@
           <t>anästhesist</t>
         </is>
       </c>
-      <c r="B159">
+      <c r="C159">
+        <v>6.67</v>
+      </c>
+      <c r="D159">
         <v>0.16</v>
       </c>
-      <c r="D159">
-        <v>6.67</v>
-      </c>
-      <c r="F159">
-        <v>6.67</v>
-      </c>
-      <c r="H159" t="inlineStr">
+      <c r="G159" t="inlineStr">
         <is>
           <t>anaesthetist</t>
         </is>
@@ -3387,10 +2875,7 @@
       <c r="C160">
         <v>6.67</v>
       </c>
-      <c r="F160">
-        <v>6.67</v>
-      </c>
-      <c r="H160" t="inlineStr">
+      <c r="G160" t="inlineStr">
         <is>
           <t>singular</t>
         </is>
@@ -3405,10 +2890,7 @@
       <c r="C161">
         <v>6.67</v>
       </c>
-      <c r="F161">
-        <v>6.67</v>
-      </c>
-      <c r="H161" t="inlineStr">
+      <c r="G161" t="inlineStr">
         <is>
           <t>elf</t>
         </is>
@@ -3423,19 +2905,13 @@
       <c r="C162">
         <v>6.67</v>
       </c>
-      <c r="F162">
-        <v>6.67</v>
-      </c>
-      <c r="H162" t="inlineStr">
+      <c r="E162">
+        <v>1.95</v>
+      </c>
+      <c r="G162" t="inlineStr">
         <is>
           <t>helicopter</t>
         </is>
-      </c>
-      <c r="I162">
-        <v>1.95</v>
-      </c>
-      <c r="J162">
-        <v>5.26</v>
       </c>
     </row>
     <row r="163">
@@ -3447,10 +2923,7 @@
       <c r="C163">
         <v>6.67</v>
       </c>
-      <c r="F163">
-        <v>6.67</v>
-      </c>
-      <c r="H163" t="inlineStr">
+      <c r="G163" t="inlineStr">
         <is>
           <t>cliff</t>
         </is>
@@ -3465,10 +2938,7 @@
       <c r="C164">
         <v>6.67</v>
       </c>
-      <c r="F164">
-        <v>6.67</v>
-      </c>
-      <c r="H164" t="inlineStr">
+      <c r="G164" t="inlineStr">
         <is>
           <t>avalanche</t>
         </is>
@@ -3483,10 +2953,7 @@
       <c r="C165">
         <v>6.67</v>
       </c>
-      <c r="F165">
-        <v>6.67</v>
-      </c>
-      <c r="H165" t="inlineStr">
+      <c r="G165" t="inlineStr">
         <is>
           <t>lotto</t>
         </is>
@@ -3501,10 +2968,7 @@
       <c r="C166">
         <v>6.67</v>
       </c>
-      <c r="F166">
-        <v>6.67</v>
-      </c>
-      <c r="H166" t="inlineStr">
+      <c r="G166" t="inlineStr">
         <is>
           <t>record</t>
         </is>
@@ -3519,10 +2983,7 @@
       <c r="C167">
         <v>6.68</v>
       </c>
-      <c r="F167">
-        <v>6.68</v>
-      </c>
-      <c r="H167" t="inlineStr">
+      <c r="G167" t="inlineStr">
         <is>
           <t>mast</t>
         </is>
@@ -3537,10 +2998,7 @@
       <c r="C168">
         <v>6.68</v>
       </c>
-      <c r="F168">
-        <v>6.68</v>
-      </c>
-      <c r="H168" t="inlineStr">
+      <c r="G168" t="inlineStr">
         <is>
           <t>envious</t>
         </is>
@@ -3555,10 +3013,7 @@
       <c r="C169">
         <v>6.68</v>
       </c>
-      <c r="F169">
-        <v>6.68</v>
-      </c>
-      <c r="H169" t="inlineStr">
+      <c r="G169" t="inlineStr">
         <is>
           <t>sense</t>
         </is>
@@ -3570,16 +3025,13 @@
           <t>stuckateur</t>
         </is>
       </c>
-      <c r="B170">
+      <c r="C170">
+        <v>6.68</v>
+      </c>
+      <c r="D170">
         <v>0.02</v>
       </c>
-      <c r="D170">
-        <v>6.68</v>
-      </c>
-      <c r="F170">
-        <v>6.68</v>
-      </c>
-      <c r="H170" t="inlineStr">
+      <c r="G170" t="inlineStr">
         <is>
           <t>plasterer</t>
         </is>
@@ -3594,10 +3046,7 @@
       <c r="C171">
         <v>6.69</v>
       </c>
-      <c r="F171">
-        <v>6.69</v>
-      </c>
-      <c r="H171" t="inlineStr">
+      <c r="G171" t="inlineStr">
         <is>
           <t>breakdown</t>
         </is>
@@ -3612,10 +3061,7 @@
       <c r="C172">
         <v>6.69</v>
       </c>
-      <c r="F172">
-        <v>6.69</v>
-      </c>
-      <c r="H172" t="inlineStr">
+      <c r="G172" t="inlineStr">
         <is>
           <t>temple</t>
         </is>
@@ -3630,10 +3076,7 @@
       <c r="C173">
         <v>6.69</v>
       </c>
-      <c r="F173">
-        <v>6.69</v>
-      </c>
-      <c r="H173" t="inlineStr">
+      <c r="G173" t="inlineStr">
         <is>
           <t>oversight</t>
         </is>
@@ -3648,10 +3091,7 @@
       <c r="C174">
         <v>6.7</v>
       </c>
-      <c r="F174">
-        <v>6.7</v>
-      </c>
-      <c r="H174" t="inlineStr">
+      <c r="G174" t="inlineStr">
         <is>
           <t>special day</t>
         </is>
@@ -3666,10 +3106,7 @@
       <c r="C175">
         <v>6.7</v>
       </c>
-      <c r="F175">
-        <v>6.7</v>
-      </c>
-      <c r="H175" t="inlineStr">
+      <c r="G175" t="inlineStr">
         <is>
           <t>terrain</t>
         </is>
@@ -3681,19 +3118,13 @@
           <t>orgel</t>
         </is>
       </c>
-      <c r="B176">
-        <v>10.14</v>
-      </c>
       <c r="C176">
         <v>6.7</v>
       </c>
       <c r="D176">
-        <v>4.65</v>
-      </c>
-      <c r="F176">
-        <v>6.7</v>
-      </c>
-      <c r="H176" t="inlineStr">
+        <v>10.14</v>
+      </c>
+      <c r="G176" t="inlineStr">
         <is>
           <t>organ</t>
         </is>
@@ -3708,10 +3139,7 @@
       <c r="C177">
         <v>6.7</v>
       </c>
-      <c r="F177">
-        <v>6.7</v>
-      </c>
-      <c r="H177" t="inlineStr">
+      <c r="G177" t="inlineStr">
         <is>
           <t>temperature</t>
         </is>
@@ -3726,10 +3154,7 @@
       <c r="C178">
         <v>6.7</v>
       </c>
-      <c r="F178">
-        <v>6.7</v>
-      </c>
-      <c r="H178" t="inlineStr">
+      <c r="G178" t="inlineStr">
         <is>
           <t>theatre</t>
         </is>
@@ -3744,10 +3169,7 @@
       <c r="C179">
         <v>6.7</v>
       </c>
-      <c r="F179">
-        <v>6.7</v>
-      </c>
-      <c r="H179" t="inlineStr">
+      <c r="G179" t="inlineStr">
         <is>
           <t>turn over</t>
         </is>
@@ -3759,16 +3181,13 @@
           <t>homöopath</t>
         </is>
       </c>
-      <c r="B180">
+      <c r="C180">
+        <v>6.7</v>
+      </c>
+      <c r="D180">
         <v>0.27</v>
       </c>
-      <c r="D180">
-        <v>6.7</v>
-      </c>
-      <c r="F180">
-        <v>6.7</v>
-      </c>
-      <c r="H180" t="inlineStr">
+      <c r="G180" t="inlineStr">
         <is>
           <t>homeopath</t>
         </is>
@@ -3783,10 +3202,7 @@
       <c r="C181">
         <v>6.71</v>
       </c>
-      <c r="F181">
-        <v>6.71</v>
-      </c>
-      <c r="H181" t="inlineStr">
+      <c r="G181" t="inlineStr">
         <is>
           <t>joint</t>
         </is>
@@ -3801,10 +3217,7 @@
       <c r="C182">
         <v>6.71</v>
       </c>
-      <c r="F182">
-        <v>6.71</v>
-      </c>
-      <c r="H182" t="inlineStr">
+      <c r="G182" t="inlineStr">
         <is>
           <t>rhyme</t>
         </is>
@@ -3819,10 +3232,7 @@
       <c r="C183">
         <v>6.71</v>
       </c>
-      <c r="F183">
-        <v>6.71</v>
-      </c>
-      <c r="H183" t="inlineStr">
+      <c r="G183" t="inlineStr">
         <is>
           <t>thrifty</t>
         </is>
@@ -3837,10 +3247,7 @@
       <c r="C184">
         <v>6.71</v>
       </c>
-      <c r="F184">
-        <v>6.71</v>
-      </c>
-      <c r="H184" t="inlineStr">
+      <c r="G184" t="inlineStr">
         <is>
           <t>impatience</t>
         </is>
@@ -3855,10 +3262,7 @@
       <c r="C185">
         <v>6.71</v>
       </c>
-      <c r="F185">
-        <v>6.71</v>
-      </c>
-      <c r="H185" t="inlineStr">
+      <c r="G185" t="inlineStr">
         <is>
           <t>prevent</t>
         </is>
@@ -3873,10 +3277,7 @@
       <c r="C186">
         <v>6.71</v>
       </c>
-      <c r="F186">
-        <v>6.71</v>
-      </c>
-      <c r="H186" t="inlineStr">
+      <c r="G186" t="inlineStr">
         <is>
           <t>female</t>
         </is>
@@ -3891,10 +3292,7 @@
       <c r="C187">
         <v>6.72</v>
       </c>
-      <c r="F187">
-        <v>6.72</v>
-      </c>
-      <c r="H187" t="inlineStr">
+      <c r="G187" t="inlineStr">
         <is>
           <t>command</t>
         </is>
@@ -3909,10 +3307,7 @@
       <c r="C188">
         <v>6.72</v>
       </c>
-      <c r="F188">
-        <v>6.72</v>
-      </c>
-      <c r="H188" t="inlineStr">
+      <c r="G188" t="inlineStr">
         <is>
           <t>wailing</t>
         </is>
@@ -3927,10 +3322,7 @@
       <c r="C189">
         <v>6.72</v>
       </c>
-      <c r="F189">
-        <v>6.72</v>
-      </c>
-      <c r="H189" t="inlineStr">
+      <c r="G189" t="inlineStr">
         <is>
           <t>throat</t>
         </is>
@@ -3945,10 +3337,7 @@
       <c r="C190">
         <v>6.72</v>
       </c>
-      <c r="F190">
-        <v>6.72</v>
-      </c>
-      <c r="H190" t="inlineStr">
+      <c r="G190" t="inlineStr">
         <is>
           <t>donate</t>
         </is>
@@ -3963,10 +3352,7 @@
       <c r="C191">
         <v>6.72</v>
       </c>
-      <c r="F191">
-        <v>6.72</v>
-      </c>
-      <c r="H191" t="inlineStr">
+      <c r="G191" t="inlineStr">
         <is>
           <t>wilderness</t>
         </is>
@@ -3981,10 +3367,7 @@
       <c r="C192">
         <v>6.73</v>
       </c>
-      <c r="F192">
-        <v>6.73</v>
-      </c>
-      <c r="H192" t="inlineStr">
+      <c r="G192" t="inlineStr">
         <is>
           <t>plot</t>
         </is>
@@ -3999,10 +3382,7 @@
       <c r="C193">
         <v>6.73</v>
       </c>
-      <c r="F193">
-        <v>6.73</v>
-      </c>
-      <c r="H193" t="inlineStr">
+      <c r="G193" t="inlineStr">
         <is>
           <t>bog</t>
         </is>
@@ -4017,10 +3397,7 @@
       <c r="C194">
         <v>6.73</v>
       </c>
-      <c r="F194">
-        <v>6.73</v>
-      </c>
-      <c r="H194" t="inlineStr">
+      <c r="G194" t="inlineStr">
         <is>
           <t>programme</t>
         </is>
@@ -4035,10 +3412,7 @@
       <c r="C195">
         <v>6.73</v>
       </c>
-      <c r="F195">
-        <v>6.73</v>
-      </c>
-      <c r="H195" t="inlineStr">
+      <c r="G195" t="inlineStr">
         <is>
           <t>twisted</t>
         </is>
@@ -4050,16 +3424,13 @@
           <t>volkswirt</t>
         </is>
       </c>
-      <c r="B196">
+      <c r="C196">
+        <v>6.74</v>
+      </c>
+      <c r="D196">
         <v>0.61</v>
       </c>
-      <c r="D196">
-        <v>6.74</v>
-      </c>
-      <c r="F196">
-        <v>6.74</v>
-      </c>
-      <c r="H196" t="inlineStr">
+      <c r="G196" t="inlineStr">
         <is>
           <t>economist</t>
         </is>
@@ -4074,10 +3445,7 @@
       <c r="C197">
         <v>6.74</v>
       </c>
-      <c r="F197">
-        <v>6.74</v>
-      </c>
-      <c r="H197" t="inlineStr">
+      <c r="G197" t="inlineStr">
         <is>
           <t>stay</t>
         </is>
@@ -4092,10 +3460,7 @@
       <c r="C198">
         <v>6.74</v>
       </c>
-      <c r="F198">
-        <v>6.74</v>
-      </c>
-      <c r="H198" t="inlineStr">
+      <c r="G198" t="inlineStr">
         <is>
           <t>appear</t>
         </is>
@@ -4110,10 +3475,7 @@
       <c r="C199">
         <v>6.74</v>
       </c>
-      <c r="F199">
-        <v>6.74</v>
-      </c>
-      <c r="H199" t="inlineStr">
+      <c r="G199" t="inlineStr">
         <is>
           <t>fill with enthusiasm</t>
         </is>
@@ -4128,10 +3490,7 @@
       <c r="C200">
         <v>6.74</v>
       </c>
-      <c r="F200">
-        <v>6.74</v>
-      </c>
-      <c r="H200" t="inlineStr">
+      <c r="G200" t="inlineStr">
         <is>
           <t>magnet</t>
         </is>
@@ -4146,10 +3505,7 @@
       <c r="C201">
         <v>6.74</v>
       </c>
-      <c r="F201">
-        <v>6.74</v>
-      </c>
-      <c r="H201" t="inlineStr">
+      <c r="G201" t="inlineStr">
         <is>
           <t>reputation</t>
         </is>
@@ -4164,10 +3520,7 @@
       <c r="C202">
         <v>6.75</v>
       </c>
-      <c r="F202">
-        <v>6.75</v>
-      </c>
-      <c r="H202" t="inlineStr">
+      <c r="G202" t="inlineStr">
         <is>
           <t>hot up</t>
         </is>
@@ -4182,10 +3535,7 @@
       <c r="C203">
         <v>6.75</v>
       </c>
-      <c r="F203">
-        <v>6.75</v>
-      </c>
-      <c r="H203" t="inlineStr">
+      <c r="G203" t="inlineStr">
         <is>
           <t>fishing</t>
         </is>
@@ -4200,10 +3550,7 @@
       <c r="C204">
         <v>6.75</v>
       </c>
-      <c r="F204">
-        <v>6.75</v>
-      </c>
-      <c r="H204" t="inlineStr">
+      <c r="G204" t="inlineStr">
         <is>
           <t>municipality</t>
         </is>
@@ -4218,10 +3565,7 @@
       <c r="C205">
         <v>6.75</v>
       </c>
-      <c r="F205">
-        <v>6.75</v>
-      </c>
-      <c r="H205" t="inlineStr">
+      <c r="G205" t="inlineStr">
         <is>
           <t>tricky</t>
         </is>
@@ -4236,10 +3580,7 @@
       <c r="C206">
         <v>6.75</v>
       </c>
-      <c r="F206">
-        <v>6.75</v>
-      </c>
-      <c r="H206" t="inlineStr">
+      <c r="G206" t="inlineStr">
         <is>
           <t>moody</t>
         </is>
@@ -4254,10 +3595,7 @@
       <c r="C207">
         <v>6.75</v>
       </c>
-      <c r="F207">
-        <v>6.75</v>
-      </c>
-      <c r="H207" t="inlineStr">
+      <c r="G207" t="inlineStr">
         <is>
           <t>stitch</t>
         </is>
@@ -4272,10 +3610,7 @@
       <c r="C208">
         <v>6.75</v>
       </c>
-      <c r="F208">
-        <v>6.75</v>
-      </c>
-      <c r="H208" t="inlineStr">
+      <c r="G208" t="inlineStr">
         <is>
           <t>works</t>
         </is>
@@ -4287,16 +3622,13 @@
           <t>thai chi</t>
         </is>
       </c>
-      <c r="B209">
+      <c r="C209">
+        <v>6.75</v>
+      </c>
+      <c r="D209">
         <v>0</v>
       </c>
-      <c r="D209">
-        <v>6.75</v>
-      </c>
-      <c r="F209">
-        <v>6.75</v>
-      </c>
-      <c r="H209" t="inlineStr">
+      <c r="G209" t="inlineStr">
         <is>
           <t>tai chi</t>
         </is>
@@ -4308,13 +3640,10 @@
           <t>soziologe</t>
         </is>
       </c>
-      <c r="D210">
+      <c r="C210">
         <v>6.75</v>
       </c>
-      <c r="F210">
-        <v>6.75</v>
-      </c>
-      <c r="H210" t="inlineStr">
+      <c r="G210" t="inlineStr">
         <is>
           <t>sociologist</t>
         </is>
@@ -4329,10 +3658,7 @@
       <c r="C211">
         <v>6.76</v>
       </c>
-      <c r="F211">
-        <v>6.76</v>
-      </c>
-      <c r="H211" t="inlineStr">
+      <c r="G211" t="inlineStr">
         <is>
           <t>gripe</t>
         </is>
@@ -4347,10 +3673,7 @@
       <c r="C212">
         <v>6.76</v>
       </c>
-      <c r="F212">
-        <v>6.76</v>
-      </c>
-      <c r="H212" t="inlineStr">
+      <c r="G212" t="inlineStr">
         <is>
           <t>joke</t>
         </is>
@@ -4365,10 +3688,7 @@
       <c r="C213">
         <v>6.76</v>
       </c>
-      <c r="F213">
-        <v>6.76</v>
-      </c>
-      <c r="H213" t="inlineStr">
+      <c r="G213" t="inlineStr">
         <is>
           <t>waiting</t>
         </is>
@@ -4380,19 +3700,13 @@
           <t>elektriker</t>
         </is>
       </c>
-      <c r="B214">
-        <v>0.96</v>
-      </c>
       <c r="C214">
         <v>6.77</v>
       </c>
       <c r="D214">
-        <v>4.4</v>
-      </c>
-      <c r="F214">
-        <v>6.77</v>
-      </c>
-      <c r="H214" t="inlineStr">
+        <v>0.96</v>
+      </c>
+      <c r="G214" t="inlineStr">
         <is>
           <t>electrician</t>
         </is>
@@ -4407,10 +3721,7 @@
       <c r="C215">
         <v>6.77</v>
       </c>
-      <c r="F215">
-        <v>6.77</v>
-      </c>
-      <c r="H215" t="inlineStr">
+      <c r="G215" t="inlineStr">
         <is>
           <t>fortress</t>
         </is>
@@ -4425,10 +3736,7 @@
       <c r="C216">
         <v>6.78</v>
       </c>
-      <c r="F216">
-        <v>6.78</v>
-      </c>
-      <c r="H216" t="inlineStr">
+      <c r="G216" t="inlineStr">
         <is>
           <t>advertisement</t>
         </is>
@@ -4443,10 +3751,7 @@
       <c r="C217">
         <v>6.79</v>
       </c>
-      <c r="F217">
-        <v>6.79</v>
-      </c>
-      <c r="H217" t="inlineStr">
+      <c r="G217" t="inlineStr">
         <is>
           <t>maple</t>
         </is>
@@ -4461,10 +3766,7 @@
       <c r="C218">
         <v>6.79</v>
       </c>
-      <c r="F218">
-        <v>6.79</v>
-      </c>
-      <c r="H218" t="inlineStr">
+      <c r="G218" t="inlineStr">
         <is>
           <t>accumulate</t>
         </is>
@@ -4479,10 +3781,7 @@
       <c r="C219">
         <v>6.79</v>
       </c>
-      <c r="F219">
-        <v>6.79</v>
-      </c>
-      <c r="H219" t="inlineStr">
+      <c r="G219" t="inlineStr">
         <is>
           <t>quantity</t>
         </is>
@@ -4497,10 +3796,7 @@
       <c r="C220">
         <v>6.79</v>
       </c>
-      <c r="F220">
-        <v>6.79</v>
-      </c>
-      <c r="H220" t="inlineStr">
+      <c r="G220" t="inlineStr">
         <is>
           <t>garland</t>
         </is>
@@ -4515,10 +3811,7 @@
       <c r="C221">
         <v>6.79</v>
       </c>
-      <c r="F221">
-        <v>6.79</v>
-      </c>
-      <c r="H221" t="inlineStr">
+      <c r="G221" t="inlineStr">
         <is>
           <t>bonnet</t>
         </is>
@@ -4533,10 +3826,7 @@
       <c r="C222">
         <v>6.79</v>
       </c>
-      <c r="F222">
-        <v>6.79</v>
-      </c>
-      <c r="H222" t="inlineStr">
+      <c r="G222" t="inlineStr">
         <is>
           <t>meal</t>
         </is>
@@ -4551,10 +3841,7 @@
       <c r="C223">
         <v>6.79</v>
       </c>
-      <c r="F223">
-        <v>6.79</v>
-      </c>
-      <c r="H223" t="inlineStr">
+      <c r="G223" t="inlineStr">
         <is>
           <t>operate</t>
         </is>
@@ -4569,10 +3856,7 @@
       <c r="C224">
         <v>6.79</v>
       </c>
-      <c r="F224">
-        <v>6.79</v>
-      </c>
-      <c r="H224" t="inlineStr">
+      <c r="G224" t="inlineStr">
         <is>
           <t>china</t>
         </is>
@@ -4587,10 +3871,7 @@
       <c r="C225">
         <v>6.79</v>
       </c>
-      <c r="F225">
-        <v>6.79</v>
-      </c>
-      <c r="H225" t="inlineStr">
+      <c r="G225" t="inlineStr">
         <is>
           <t>syrup</t>
         </is>
@@ -4605,10 +3886,7 @@
       <c r="C226">
         <v>6.79</v>
       </c>
-      <c r="F226">
-        <v>6.79</v>
-      </c>
-      <c r="H226" t="inlineStr">
+      <c r="G226" t="inlineStr">
         <is>
           <t>villa</t>
         </is>
@@ -4623,10 +3901,7 @@
       <c r="C227">
         <v>6.8</v>
       </c>
-      <c r="F227">
-        <v>6.8</v>
-      </c>
-      <c r="H227" t="inlineStr">
+      <c r="G227" t="inlineStr">
         <is>
           <t>dropping</t>
         </is>
@@ -4641,10 +3916,7 @@
       <c r="C228">
         <v>6.8</v>
       </c>
-      <c r="F228">
-        <v>6.8</v>
-      </c>
-      <c r="H228" t="inlineStr">
+      <c r="G228" t="inlineStr">
         <is>
           <t>skip</t>
         </is>
@@ -4659,10 +3931,7 @@
       <c r="C229">
         <v>6.8</v>
       </c>
-      <c r="F229">
-        <v>6.8</v>
-      </c>
-      <c r="H229" t="inlineStr">
+      <c r="G229" t="inlineStr">
         <is>
           <t>triplet</t>
         </is>
@@ -4677,10 +3946,7 @@
       <c r="C230">
         <v>6.8</v>
       </c>
-      <c r="F230">
-        <v>6.8</v>
-      </c>
-      <c r="H230" t="inlineStr">
+      <c r="G230" t="inlineStr">
         <is>
           <t>solemn</t>
         </is>
@@ -4695,10 +3961,7 @@
       <c r="C231">
         <v>6.8</v>
       </c>
-      <c r="F231">
-        <v>6.8</v>
-      </c>
-      <c r="H231" t="inlineStr">
+      <c r="G231" t="inlineStr">
         <is>
           <t>hobby</t>
         </is>
@@ -4713,10 +3976,7 @@
       <c r="C232">
         <v>6.8</v>
       </c>
-      <c r="F232">
-        <v>6.8</v>
-      </c>
-      <c r="H232" t="inlineStr">
+      <c r="G232" t="inlineStr">
         <is>
           <t>lexicon</t>
         </is>
@@ -4731,10 +3991,7 @@
       <c r="C233">
         <v>6.8</v>
       </c>
-      <c r="F233">
-        <v>6.8</v>
-      </c>
-      <c r="H233" t="inlineStr">
+      <c r="G233" t="inlineStr">
         <is>
           <t>ramp</t>
         </is>
@@ -4749,10 +4006,7 @@
       <c r="C234">
         <v>6.8</v>
       </c>
-      <c r="F234">
-        <v>6.8</v>
-      </c>
-      <c r="H234" t="inlineStr">
+      <c r="G234" t="inlineStr">
         <is>
           <t>lullaby</t>
         </is>
@@ -4764,13 +4018,10 @@
           <t>katamaransegeln</t>
         </is>
       </c>
-      <c r="D235">
+      <c r="C235">
         <v>6.8</v>
       </c>
-      <c r="F235">
-        <v>6.8</v>
-      </c>
-      <c r="H235" t="inlineStr">
+      <c r="G235" t="inlineStr">
         <is>
           <t>catamaran sailing</t>
         </is>
@@ -4785,10 +4036,7 @@
       <c r="C236">
         <v>6.81</v>
       </c>
-      <c r="F236">
-        <v>6.81</v>
-      </c>
-      <c r="H236" t="inlineStr">
+      <c r="G236" t="inlineStr">
         <is>
           <t>herring</t>
         </is>
@@ -4803,10 +4051,7 @@
       <c r="C237">
         <v>6.81</v>
       </c>
-      <c r="F237">
-        <v>6.81</v>
-      </c>
-      <c r="H237" t="inlineStr">
+      <c r="G237" t="inlineStr">
         <is>
           <t>lava</t>
         </is>
@@ -4821,10 +4066,7 @@
       <c r="C238">
         <v>6.81</v>
       </c>
-      <c r="F238">
-        <v>6.81</v>
-      </c>
-      <c r="H238" t="inlineStr">
+      <c r="G238" t="inlineStr">
         <is>
           <t>embarrassing</t>
         </is>
@@ -4839,10 +4081,7 @@
       <c r="C239">
         <v>6.81</v>
       </c>
-      <c r="F239">
-        <v>6.81</v>
-      </c>
-      <c r="H239" t="inlineStr">
+      <c r="G239" t="inlineStr">
         <is>
           <t>weakness</t>
         </is>
@@ -4854,16 +4093,13 @@
           <t>physalis</t>
         </is>
       </c>
-      <c r="B240">
+      <c r="C240">
+        <v>6.81</v>
+      </c>
+      <c r="D240">
         <v>0.07000000000000001</v>
       </c>
-      <c r="D240">
-        <v>6.81</v>
-      </c>
-      <c r="F240">
-        <v>6.81</v>
-      </c>
-      <c r="H240" t="inlineStr">
+      <c r="G240" t="inlineStr">
         <is>
           <t>physalis</t>
         </is>
@@ -4878,10 +4114,7 @@
       <c r="C241">
         <v>6.82</v>
       </c>
-      <c r="F241">
-        <v>6.82</v>
-      </c>
-      <c r="H241" t="inlineStr">
+      <c r="G241" t="inlineStr">
         <is>
           <t>astronaut</t>
         </is>
@@ -4896,10 +4129,7 @@
       <c r="C242">
         <v>6.82</v>
       </c>
-      <c r="F242">
-        <v>6.82</v>
-      </c>
-      <c r="H242" t="inlineStr">
+      <c r="G242" t="inlineStr">
         <is>
           <t>car radio</t>
         </is>
@@ -4914,10 +4144,7 @@
       <c r="C243">
         <v>6.82</v>
       </c>
-      <c r="F243">
-        <v>6.82</v>
-      </c>
-      <c r="H243" t="inlineStr">
+      <c r="G243" t="inlineStr">
         <is>
           <t>champion</t>
         </is>
@@ -4932,10 +4159,7 @@
       <c r="C244">
         <v>6.83</v>
       </c>
-      <c r="F244">
-        <v>6.83</v>
-      </c>
-      <c r="H244" t="inlineStr">
+      <c r="G244" t="inlineStr">
         <is>
           <t>recording</t>
         </is>
@@ -4950,10 +4174,7 @@
       <c r="C245">
         <v>6.83</v>
       </c>
-      <c r="F245">
-        <v>6.83</v>
-      </c>
-      <c r="H245" t="inlineStr">
+      <c r="G245" t="inlineStr">
         <is>
           <t>cash</t>
         </is>
@@ -4968,10 +4189,7 @@
       <c r="C246">
         <v>6.83</v>
       </c>
-      <c r="F246">
-        <v>6.83</v>
-      </c>
-      <c r="H246" t="inlineStr">
+      <c r="G246" t="inlineStr">
         <is>
           <t>denote</t>
         </is>
@@ -4986,10 +4204,7 @@
       <c r="C247">
         <v>6.83</v>
       </c>
-      <c r="F247">
-        <v>6.83</v>
-      </c>
-      <c r="H247" t="inlineStr">
+      <c r="G247" t="inlineStr">
         <is>
           <t>boss</t>
         </is>
@@ -5004,10 +4219,7 @@
       <c r="C248">
         <v>6.83</v>
       </c>
-      <c r="F248">
-        <v>6.83</v>
-      </c>
-      <c r="H248" t="inlineStr">
+      <c r="G248" t="inlineStr">
         <is>
           <t>facial expression</t>
         </is>
@@ -5022,10 +4234,7 @@
       <c r="C249">
         <v>6.83</v>
       </c>
-      <c r="F249">
-        <v>6.83</v>
-      </c>
-      <c r="H249" t="inlineStr">
+      <c r="G249" t="inlineStr">
         <is>
           <t>partner</t>
         </is>
@@ -5040,10 +4249,7 @@
       <c r="C250">
         <v>6.83</v>
       </c>
-      <c r="F250">
-        <v>6.83</v>
-      </c>
-      <c r="H250" t="inlineStr">
+      <c r="G250" t="inlineStr">
         <is>
           <t>pool</t>
         </is>
@@ -5055,16 +4261,13 @@
           <t>diätassistent</t>
         </is>
       </c>
-      <c r="B251">
+      <c r="C251">
+        <v>6.83</v>
+      </c>
+      <c r="D251">
         <v>0.01</v>
       </c>
-      <c r="D251">
-        <v>6.83</v>
-      </c>
-      <c r="F251">
-        <v>6.83</v>
-      </c>
-      <c r="H251" t="inlineStr">
+      <c r="G251" t="inlineStr">
         <is>
           <t>dietician</t>
         </is>
@@ -5079,10 +4282,7 @@
       <c r="C252">
         <v>6.84</v>
       </c>
-      <c r="F252">
-        <v>6.84</v>
-      </c>
-      <c r="H252" t="inlineStr">
+      <c r="G252" t="inlineStr">
         <is>
           <t>value</t>
         </is>
@@ -5097,10 +4297,7 @@
       <c r="C253">
         <v>6.84</v>
       </c>
-      <c r="F253">
-        <v>6.84</v>
-      </c>
-      <c r="H253" t="inlineStr">
+      <c r="G253" t="inlineStr">
         <is>
           <t>folder</t>
         </is>
@@ -5112,13 +4309,10 @@
           <t>eventmanager</t>
         </is>
       </c>
-      <c r="D254">
+      <c r="C254">
         <v>6.84</v>
       </c>
-      <c r="F254">
-        <v>6.84</v>
-      </c>
-      <c r="H254" t="inlineStr">
+      <c r="G254" t="inlineStr">
         <is>
           <t>event manager</t>
         </is>
@@ -5130,13 +4324,10 @@
           <t>ergotherapeut</t>
         </is>
       </c>
-      <c r="D255">
+      <c r="C255">
         <v>6.84</v>
       </c>
-      <c r="F255">
-        <v>6.84</v>
-      </c>
-      <c r="H255" t="inlineStr">
+      <c r="G255" t="inlineStr">
         <is>
           <t>occupational therapist</t>
         </is>
@@ -5151,10 +4342,7 @@
       <c r="C256">
         <v>6.85</v>
       </c>
-      <c r="F256">
-        <v>6.85</v>
-      </c>
-      <c r="H256" t="inlineStr">
+      <c r="G256" t="inlineStr">
         <is>
           <t>mark</t>
         </is>
@@ -5169,10 +4357,7 @@
       <c r="C257">
         <v>6.85</v>
       </c>
-      <c r="F257">
-        <v>6.85</v>
-      </c>
-      <c r="H257" t="inlineStr">
+      <c r="G257" t="inlineStr">
         <is>
           <t>finish speaking</t>
         </is>
@@ -5187,10 +4372,7 @@
       <c r="C258">
         <v>6.85</v>
       </c>
-      <c r="F258">
-        <v>6.85</v>
-      </c>
-      <c r="H258" t="inlineStr">
+      <c r="G258" t="inlineStr">
         <is>
           <t>pub</t>
         </is>
@@ -5202,13 +4384,10 @@
           <t>nordic-walking</t>
         </is>
       </c>
-      <c r="D259">
+      <c r="C259">
         <v>6.85</v>
       </c>
-      <c r="F259">
-        <v>6.85</v>
-      </c>
-      <c r="H259" t="inlineStr">
+      <c r="G259" t="inlineStr">
         <is>
           <t>nordic walking</t>
         </is>
@@ -5220,16 +4399,13 @@
           <t>betriebswirt</t>
         </is>
       </c>
-      <c r="B260">
+      <c r="C260">
+        <v>6.85</v>
+      </c>
+      <c r="D260">
         <v>0.48</v>
       </c>
-      <c r="D260">
-        <v>6.85</v>
-      </c>
-      <c r="F260">
-        <v>6.85</v>
-      </c>
-      <c r="H260" t="inlineStr">
+      <c r="G260" t="inlineStr">
         <is>
           <t>business economist</t>
         </is>
@@ -5241,13 +4417,10 @@
           <t>kommunikationsassistent</t>
         </is>
       </c>
-      <c r="D261">
+      <c r="C261">
         <v>6.85</v>
       </c>
-      <c r="F261">
-        <v>6.85</v>
-      </c>
-      <c r="H261" t="inlineStr">
+      <c r="G261" t="inlineStr">
         <is>
           <t>communications assistant</t>
         </is>
@@ -5262,10 +4435,7 @@
       <c r="C262">
         <v>6.87</v>
       </c>
-      <c r="F262">
-        <v>6.87</v>
-      </c>
-      <c r="H262" t="inlineStr">
+      <c r="G262" t="inlineStr">
         <is>
           <t>be exposed</t>
         </is>
@@ -5280,10 +4450,7 @@
       <c r="C263">
         <v>6.87</v>
       </c>
-      <c r="F263">
-        <v>6.87</v>
-      </c>
-      <c r="H263" t="inlineStr">
+      <c r="G263" t="inlineStr">
         <is>
           <t>payment</t>
         </is>
@@ -5298,10 +4465,7 @@
       <c r="C264">
         <v>6.88</v>
       </c>
-      <c r="F264">
-        <v>6.88</v>
-      </c>
-      <c r="H264" t="inlineStr">
+      <c r="G264" t="inlineStr">
         <is>
           <t>compartment</t>
         </is>
@@ -5313,19 +4477,13 @@
           <t>ballett</t>
         </is>
       </c>
-      <c r="B265">
-        <v>7.22</v>
-      </c>
       <c r="C265">
         <v>6.88</v>
       </c>
       <c r="D265">
-        <v>4.15</v>
-      </c>
-      <c r="F265">
-        <v>6.88</v>
-      </c>
-      <c r="H265" t="inlineStr">
+        <v>7.22</v>
+      </c>
+      <c r="G265" t="inlineStr">
         <is>
           <t>ballet</t>
         </is>
@@ -5340,10 +4498,7 @@
       <c r="C266">
         <v>6.88</v>
       </c>
-      <c r="F266">
-        <v>6.88</v>
-      </c>
-      <c r="H266" t="inlineStr">
+      <c r="G266" t="inlineStr">
         <is>
           <t>report</t>
         </is>
@@ -5358,10 +4513,7 @@
       <c r="C267">
         <v>6.88</v>
       </c>
-      <c r="F267">
-        <v>6.88</v>
-      </c>
-      <c r="H267" t="inlineStr">
+      <c r="G267" t="inlineStr">
         <is>
           <t>chance</t>
         </is>
@@ -5373,16 +4525,13 @@
           <t>publizist</t>
         </is>
       </c>
-      <c r="B268">
+      <c r="C268">
+        <v>6.89</v>
+      </c>
+      <c r="D268">
         <v>3.24</v>
       </c>
-      <c r="D268">
-        <v>6.89</v>
-      </c>
-      <c r="F268">
-        <v>6.89</v>
-      </c>
-      <c r="H268" t="inlineStr">
+      <c r="G268" t="inlineStr">
         <is>
           <t>publicist</t>
         </is>
@@ -5397,10 +4546,7 @@
       <c r="C269">
         <v>6.89</v>
       </c>
-      <c r="F269">
-        <v>6.89</v>
-      </c>
-      <c r="H269" t="inlineStr">
+      <c r="G269" t="inlineStr">
         <is>
           <t>allergy</t>
         </is>
@@ -5415,10 +4561,7 @@
       <c r="C270">
         <v>6.89</v>
       </c>
-      <c r="F270">
-        <v>6.89</v>
-      </c>
-      <c r="H270" t="inlineStr">
+      <c r="G270" t="inlineStr">
         <is>
           <t>pop song</t>
         </is>
@@ -5433,10 +4576,7 @@
       <c r="C271">
         <v>6.89</v>
       </c>
-      <c r="F271">
-        <v>6.89</v>
-      </c>
-      <c r="H271" t="inlineStr">
+      <c r="G271" t="inlineStr">
         <is>
           <t>drum roll</t>
         </is>
@@ -5451,10 +4591,7 @@
       <c r="C272">
         <v>6.9</v>
       </c>
-      <c r="F272">
-        <v>6.9</v>
-      </c>
-      <c r="H272" t="inlineStr">
+      <c r="G272" t="inlineStr">
         <is>
           <t>splendid</t>
         </is>
@@ -5466,13 +4603,10 @@
           <t>steuerfachangestellter</t>
         </is>
       </c>
-      <c r="D273">
+      <c r="C273">
         <v>6.9</v>
       </c>
-      <c r="F273">
-        <v>6.9</v>
-      </c>
-      <c r="H273" t="inlineStr">
+      <c r="G273" t="inlineStr">
         <is>
           <t>assistant tax consultant</t>
         </is>
@@ -5484,16 +4618,13 @@
           <t>kardiologe</t>
         </is>
       </c>
-      <c r="B274">
+      <c r="C274">
+        <v>6.9</v>
+      </c>
+      <c r="D274">
         <v>0.02</v>
       </c>
-      <c r="D274">
-        <v>6.9</v>
-      </c>
-      <c r="F274">
-        <v>6.9</v>
-      </c>
-      <c r="H274" t="inlineStr">
+      <c r="G274" t="inlineStr">
         <is>
           <t>cardiologist</t>
         </is>
@@ -5505,16 +4636,13 @@
           <t>radiologe</t>
         </is>
       </c>
-      <c r="B275">
+      <c r="C275">
+        <v>6.9</v>
+      </c>
+      <c r="D275">
         <v>0.02</v>
       </c>
-      <c r="D275">
-        <v>6.9</v>
-      </c>
-      <c r="F275">
-        <v>6.9</v>
-      </c>
-      <c r="H275" t="inlineStr">
+      <c r="G275" t="inlineStr">
         <is>
           <t>radiologist</t>
         </is>
@@ -5526,19 +4654,13 @@
           <t>brokkoli</t>
         </is>
       </c>
-      <c r="B276">
-        <v>0.17</v>
-      </c>
       <c r="C276">
         <v>6.91</v>
       </c>
       <c r="D276">
-        <v>5.53</v>
-      </c>
-      <c r="F276">
-        <v>6.91</v>
-      </c>
-      <c r="H276" t="inlineStr">
+        <v>0.17</v>
+      </c>
+      <c r="G276" t="inlineStr">
         <is>
           <t>broccoli</t>
         </is>
@@ -5553,10 +4675,7 @@
       <c r="C277">
         <v>6.92</v>
       </c>
-      <c r="F277">
-        <v>6.92</v>
-      </c>
-      <c r="H277" t="inlineStr">
+      <c r="G277" t="inlineStr">
         <is>
           <t>loudspeaker</t>
         </is>
@@ -5571,10 +4690,7 @@
       <c r="C278">
         <v>6.92</v>
       </c>
-      <c r="F278">
-        <v>6.92</v>
-      </c>
-      <c r="H278" t="inlineStr">
+      <c r="G278" t="inlineStr">
         <is>
           <t>region</t>
         </is>
@@ -5589,10 +4705,7 @@
       <c r="C279">
         <v>6.92</v>
       </c>
-      <c r="F279">
-        <v>6.92</v>
-      </c>
-      <c r="H279" t="inlineStr">
+      <c r="G279" t="inlineStr">
         <is>
           <t>nephew</t>
         </is>
@@ -5607,10 +4720,7 @@
       <c r="C280">
         <v>6.92</v>
       </c>
-      <c r="F280">
-        <v>6.92</v>
-      </c>
-      <c r="H280" t="inlineStr">
+      <c r="G280" t="inlineStr">
         <is>
           <t>paradise</t>
         </is>
@@ -5625,10 +4735,7 @@
       <c r="C281">
         <v>6.92</v>
       </c>
-      <c r="F281">
-        <v>6.92</v>
-      </c>
-      <c r="H281" t="inlineStr">
+      <c r="G281" t="inlineStr">
         <is>
           <t>rust</t>
         </is>
@@ -5643,10 +4750,7 @@
       <c r="C282">
         <v>6.92</v>
       </c>
-      <c r="F282">
-        <v>6.92</v>
-      </c>
-      <c r="H282" t="inlineStr">
+      <c r="G282" t="inlineStr">
         <is>
           <t>speechless</t>
         </is>
@@ -5661,10 +4765,7 @@
       <c r="C283">
         <v>6.93</v>
       </c>
-      <c r="F283">
-        <v>6.93</v>
-      </c>
-      <c r="H283" t="inlineStr">
+      <c r="G283" t="inlineStr">
         <is>
           <t>proof</t>
         </is>
@@ -5679,10 +4780,7 @@
       <c r="C284">
         <v>6.93</v>
       </c>
-      <c r="F284">
-        <v>6.93</v>
-      </c>
-      <c r="H284" t="inlineStr">
+      <c r="G284" t="inlineStr">
         <is>
           <t>contain</t>
         </is>
@@ -5697,10 +4795,7 @@
       <c r="C285">
         <v>6.93</v>
       </c>
-      <c r="F285">
-        <v>6.93</v>
-      </c>
-      <c r="H285" t="inlineStr">
+      <c r="G285" t="inlineStr">
         <is>
           <t>concert</t>
         </is>
@@ -5715,10 +4810,7 @@
       <c r="C286">
         <v>6.93</v>
       </c>
-      <c r="F286">
-        <v>6.93</v>
-      </c>
-      <c r="H286" t="inlineStr">
+      <c r="G286" t="inlineStr">
         <is>
           <t>tweezers</t>
         </is>
@@ -5733,10 +4825,7 @@
       <c r="C287">
         <v>6.93</v>
       </c>
-      <c r="F287">
-        <v>6.93</v>
-      </c>
-      <c r="H287" t="inlineStr">
+      <c r="G287" t="inlineStr">
         <is>
           <t>lower</t>
         </is>
@@ -5751,10 +4840,7 @@
       <c r="C288">
         <v>6.94</v>
       </c>
-      <c r="F288">
-        <v>6.94</v>
-      </c>
-      <c r="H288" t="inlineStr">
+      <c r="G288" t="inlineStr">
         <is>
           <t>lungs</t>
         </is>
@@ -5769,10 +4855,7 @@
       <c r="C289">
         <v>6.94</v>
       </c>
-      <c r="F289">
-        <v>6.94</v>
-      </c>
-      <c r="H289" t="inlineStr">
+      <c r="G289" t="inlineStr">
         <is>
           <t>listless</t>
         </is>
@@ -5787,10 +4870,7 @@
       <c r="C290">
         <v>6.94</v>
       </c>
-      <c r="F290">
-        <v>6.94</v>
-      </c>
-      <c r="H290" t="inlineStr">
+      <c r="G290" t="inlineStr">
         <is>
           <t>without trace</t>
         </is>
@@ -5805,10 +4885,7 @@
       <c r="C291">
         <v>6.94</v>
       </c>
-      <c r="F291">
-        <v>6.94</v>
-      </c>
-      <c r="H291" t="inlineStr">
+      <c r="G291" t="inlineStr">
         <is>
           <t>conversation</t>
         </is>
@@ -5820,16 +4897,13 @@
           <t>broker</t>
         </is>
       </c>
-      <c r="B292">
+      <c r="C292">
+        <v>6.94</v>
+      </c>
+      <c r="D292">
         <v>0.25</v>
       </c>
-      <c r="D292">
-        <v>6.94</v>
-      </c>
-      <c r="F292">
-        <v>6.94</v>
-      </c>
-      <c r="H292" t="inlineStr">
+      <c r="G292" t="inlineStr">
         <is>
           <t>broker</t>
         </is>
@@ -5841,13 +4915,10 @@
           <t>onkologe</t>
         </is>
       </c>
-      <c r="D293">
+      <c r="C293">
         <v>6.95</v>
       </c>
-      <c r="F293">
-        <v>6.95</v>
-      </c>
-      <c r="H293" t="inlineStr">
+      <c r="G293" t="inlineStr">
         <is>
           <t>oncologist</t>
         </is>
@@ -5862,10 +4933,7 @@
       <c r="C294">
         <v>6.95</v>
       </c>
-      <c r="F294">
-        <v>6.95</v>
-      </c>
-      <c r="H294" t="inlineStr">
+      <c r="G294" t="inlineStr">
         <is>
           <t>dent</t>
         </is>
@@ -5880,10 +4948,7 @@
       <c r="C295">
         <v>6.95</v>
       </c>
-      <c r="F295">
-        <v>6.95</v>
-      </c>
-      <c r="H295" t="inlineStr">
+      <c r="G295" t="inlineStr">
         <is>
           <t>impression</t>
         </is>
@@ -5898,10 +4963,7 @@
       <c r="C296">
         <v>6.95</v>
       </c>
-      <c r="F296">
-        <v>6.95</v>
-      </c>
-      <c r="H296" t="inlineStr">
+      <c r="G296" t="inlineStr">
         <is>
           <t>be received</t>
         </is>
@@ -5916,10 +4978,7 @@
       <c r="C297">
         <v>6.95</v>
       </c>
-      <c r="F297">
-        <v>6.95</v>
-      </c>
-      <c r="H297" t="inlineStr">
+      <c r="G297" t="inlineStr">
         <is>
           <t>flounder</t>
         </is>
@@ -5934,10 +4993,7 @@
       <c r="C298">
         <v>6.95</v>
       </c>
-      <c r="F298">
-        <v>6.95</v>
-      </c>
-      <c r="H298" t="inlineStr">
+      <c r="G298" t="inlineStr">
         <is>
           <t>often</t>
         </is>
@@ -5952,10 +5008,7 @@
       <c r="C299">
         <v>6.95</v>
       </c>
-      <c r="F299">
-        <v>6.95</v>
-      </c>
-      <c r="H299" t="inlineStr">
+      <c r="G299" t="inlineStr">
         <is>
           <t>pyramid</t>
         </is>
@@ -5967,19 +5020,13 @@
           <t>fähre</t>
         </is>
       </c>
-      <c r="B300">
-        <v>2.15</v>
-      </c>
       <c r="C300">
         <v>6.96</v>
       </c>
       <c r="D300">
-        <v>3.9</v>
-      </c>
-      <c r="F300">
-        <v>6.96</v>
-      </c>
-      <c r="H300" t="inlineStr">
+        <v>2.15</v>
+      </c>
+      <c r="G300" t="inlineStr">
         <is>
           <t>ferry</t>
         </is>
@@ -5994,10 +5041,7 @@
       <c r="C301">
         <v>6.96</v>
       </c>
-      <c r="F301">
-        <v>6.96</v>
-      </c>
-      <c r="H301" t="inlineStr">
+      <c r="G301" t="inlineStr">
         <is>
           <t>continue</t>
         </is>
@@ -6012,10 +5056,7 @@
       <c r="C302">
         <v>6.96</v>
       </c>
-      <c r="F302">
-        <v>6.96</v>
-      </c>
-      <c r="H302" t="inlineStr">
+      <c r="G302" t="inlineStr">
         <is>
           <t>deliver</t>
         </is>
@@ -6027,19 +5068,13 @@
           <t>schach</t>
         </is>
       </c>
-      <c r="B303">
-        <v>4.5</v>
-      </c>
       <c r="C303">
         <v>6.96</v>
       </c>
       <c r="D303">
-        <v>4</v>
-      </c>
-      <c r="F303">
-        <v>6.96</v>
-      </c>
-      <c r="H303" t="inlineStr">
+        <v>4.5</v>
+      </c>
+      <c r="G303" t="inlineStr">
         <is>
           <t>chess</t>
         </is>
@@ -6054,10 +5089,7 @@
       <c r="C304">
         <v>6.96</v>
       </c>
-      <c r="F304">
-        <v>6.96</v>
-      </c>
-      <c r="H304" t="inlineStr">
+      <c r="G304" t="inlineStr">
         <is>
           <t>test</t>
         </is>
@@ -6072,10 +5104,7 @@
       <c r="C305">
         <v>7</v>
       </c>
-      <c r="F305">
-        <v>7</v>
-      </c>
-      <c r="H305" t="inlineStr">
+      <c r="G305" t="inlineStr">
         <is>
           <t>take off</t>
         </is>
@@ -6090,10 +5119,7 @@
       <c r="C306">
         <v>7</v>
       </c>
-      <c r="F306">
-        <v>7</v>
-      </c>
-      <c r="H306" t="inlineStr">
+      <c r="G306" t="inlineStr">
         <is>
           <t>premonition</t>
         </is>
@@ -6108,10 +5134,7 @@
       <c r="C307">
         <v>7</v>
       </c>
-      <c r="F307">
-        <v>7</v>
-      </c>
-      <c r="H307" t="inlineStr">
+      <c r="G307" t="inlineStr">
         <is>
           <t>understand</t>
         </is>
@@ -6126,10 +5149,7 @@
       <c r="C308">
         <v>7</v>
       </c>
-      <c r="F308">
-        <v>7</v>
-      </c>
-      <c r="H308" t="inlineStr">
+      <c r="G308" t="inlineStr">
         <is>
           <t>arise</t>
         </is>
@@ -6144,10 +5164,7 @@
       <c r="C309">
         <v>7</v>
       </c>
-      <c r="F309">
-        <v>7</v>
-      </c>
-      <c r="H309" t="inlineStr">
+      <c r="G309" t="inlineStr">
         <is>
           <t>complete</t>
         </is>
@@ -6162,10 +5179,7 @@
       <c r="C310">
         <v>7</v>
       </c>
-      <c r="F310">
-        <v>7</v>
-      </c>
-      <c r="H310" t="inlineStr">
+      <c r="G310" t="inlineStr">
         <is>
           <t>substitute</t>
         </is>
@@ -6180,10 +5194,7 @@
       <c r="C311">
         <v>7</v>
       </c>
-      <c r="F311">
-        <v>7</v>
-      </c>
-      <c r="H311" t="inlineStr">
+      <c r="G311" t="inlineStr">
         <is>
           <t>tide</t>
         </is>
@@ -6198,10 +5209,7 @@
       <c r="C312">
         <v>7</v>
       </c>
-      <c r="F312">
-        <v>7</v>
-      </c>
-      <c r="H312" t="inlineStr">
+      <c r="G312" t="inlineStr">
         <is>
           <t>foil</t>
         </is>
@@ -6216,10 +5224,7 @@
       <c r="C313">
         <v>7</v>
       </c>
-      <c r="F313">
-        <v>7</v>
-      </c>
-      <c r="H313" t="inlineStr">
+      <c r="G313" t="inlineStr">
         <is>
           <t>volunteer</t>
         </is>
@@ -6234,10 +5239,7 @@
       <c r="C314">
         <v>7</v>
       </c>
-      <c r="F314">
-        <v>7</v>
-      </c>
-      <c r="H314" t="inlineStr">
+      <c r="G314" t="inlineStr">
         <is>
           <t>thought</t>
         </is>
@@ -6252,10 +5254,7 @@
       <c r="C315">
         <v>7</v>
       </c>
-      <c r="F315">
-        <v>7</v>
-      </c>
-      <c r="H315" t="inlineStr">
+      <c r="G315" t="inlineStr">
         <is>
           <t>error</t>
         </is>
@@ -6270,19 +5269,13 @@
       <c r="C316">
         <v>7</v>
       </c>
-      <c r="F316">
-        <v>7</v>
-      </c>
-      <c r="H316" t="inlineStr">
+      <c r="E316">
+        <v>4.71</v>
+      </c>
+      <c r="G316" t="inlineStr">
         <is>
           <t>boy</t>
         </is>
-      </c>
-      <c r="I316">
-        <v>4.71</v>
-      </c>
-      <c r="J316">
-        <v>3</v>
       </c>
     </row>
     <row r="317">
@@ -6294,10 +5287,7 @@
       <c r="C317">
         <v>7</v>
       </c>
-      <c r="F317">
-        <v>7</v>
-      </c>
-      <c r="H317" t="inlineStr">
+      <c r="G317" t="inlineStr">
         <is>
           <t>control</t>
         </is>
@@ -6312,10 +5302,7 @@
       <c r="C318">
         <v>7</v>
       </c>
-      <c r="F318">
-        <v>7</v>
-      </c>
-      <c r="H318" t="inlineStr">
+      <c r="G318" t="inlineStr">
         <is>
           <t>achievement</t>
         </is>
@@ -6327,19 +5314,13 @@
           <t>pelikan</t>
         </is>
       </c>
-      <c r="B319">
-        <v>0.7</v>
-      </c>
       <c r="C319">
         <v>7</v>
       </c>
       <c r="D319">
-        <v>3.9</v>
-      </c>
-      <c r="F319">
-        <v>7</v>
-      </c>
-      <c r="H319" t="inlineStr">
+        <v>0.7</v>
+      </c>
+      <c r="G319" t="inlineStr">
         <is>
           <t>pelican</t>
         </is>
@@ -6354,10 +5335,7 @@
       <c r="C320">
         <v>7</v>
       </c>
-      <c r="F320">
-        <v>7</v>
-      </c>
-      <c r="H320" t="inlineStr">
+      <c r="G320" t="inlineStr">
         <is>
           <t>quiz</t>
         </is>
@@ -6369,19 +5347,13 @@
           <t>saxophon</t>
         </is>
       </c>
-      <c r="B321">
-        <v>0.92</v>
-      </c>
       <c r="C321">
         <v>7</v>
       </c>
       <c r="D321">
-        <v>4.45</v>
-      </c>
-      <c r="F321">
-        <v>7</v>
-      </c>
-      <c r="H321" t="inlineStr">
+        <v>0.92</v>
+      </c>
+      <c r="G321" t="inlineStr">
         <is>
           <t>saxophone</t>
         </is>
@@ -6396,10 +5368,7 @@
       <c r="C322">
         <v>7</v>
       </c>
-      <c r="F322">
-        <v>7</v>
-      </c>
-      <c r="H322" t="inlineStr">
+      <c r="G322" t="inlineStr">
         <is>
           <t>seasick</t>
         </is>
@@ -6411,19 +5380,13 @@
           <t>tacker</t>
         </is>
       </c>
-      <c r="B323">
-        <v>0.1</v>
-      </c>
       <c r="C323">
         <v>7</v>
       </c>
       <c r="D323">
-        <v>5.58</v>
-      </c>
-      <c r="F323">
-        <v>7</v>
-      </c>
-      <c r="H323" t="inlineStr">
+        <v>0.1</v>
+      </c>
+      <c r="G323" t="inlineStr">
         <is>
           <t>stapler</t>
         </is>
@@ -6438,10 +5401,7 @@
       <c r="C324">
         <v>7.04</v>
       </c>
-      <c r="F324">
-        <v>7.04</v>
-      </c>
-      <c r="H324" t="inlineStr">
+      <c r="G324" t="inlineStr">
         <is>
           <t>interest</t>
         </is>
@@ -6456,10 +5416,7 @@
       <c r="C325">
         <v>7.04</v>
       </c>
-      <c r="F325">
-        <v>7.04</v>
-      </c>
-      <c r="H325" t="inlineStr">
+      <c r="G325" t="inlineStr">
         <is>
           <t>march</t>
         </is>
@@ -6474,10 +5431,7 @@
       <c r="C326">
         <v>7.04</v>
       </c>
-      <c r="F326">
-        <v>7.04</v>
-      </c>
-      <c r="H326" t="inlineStr">
+      <c r="G326" t="inlineStr">
         <is>
           <t>big seller</t>
         </is>
@@ -6492,10 +5446,7 @@
       <c r="C327">
         <v>7.04</v>
       </c>
-      <c r="F327">
-        <v>7.04</v>
-      </c>
-      <c r="H327" t="inlineStr">
+      <c r="G327" t="inlineStr">
         <is>
           <t>weird</t>
         </is>
@@ -6510,10 +5461,7 @@
       <c r="C328">
         <v>7.04</v>
       </c>
-      <c r="F328">
-        <v>7.04</v>
-      </c>
-      <c r="H328" t="inlineStr">
+      <c r="G328" t="inlineStr">
         <is>
           <t>talking</t>
         </is>
@@ -6528,10 +5476,7 @@
       <c r="C329">
         <v>7.04</v>
       </c>
-      <c r="F329">
-        <v>7.04</v>
-      </c>
-      <c r="H329" t="inlineStr">
+      <c r="G329" t="inlineStr">
         <is>
           <t>verse</t>
         </is>
@@ -6546,10 +5491,7 @@
       <c r="C330">
         <v>7.05</v>
       </c>
-      <c r="F330">
-        <v>7.05</v>
-      </c>
-      <c r="H330" t="inlineStr">
+      <c r="G330" t="inlineStr">
         <is>
           <t>instruction</t>
         </is>
@@ -6564,10 +5506,7 @@
       <c r="C331">
         <v>7.05</v>
       </c>
-      <c r="F331">
-        <v>7.05</v>
-      </c>
-      <c r="H331" t="inlineStr">
+      <c r="G331" t="inlineStr">
         <is>
           <t>finishing time</t>
         </is>
@@ -6582,10 +5521,7 @@
       <c r="C332">
         <v>7.05</v>
       </c>
-      <c r="F332">
-        <v>7.05</v>
-      </c>
-      <c r="H332" t="inlineStr">
+      <c r="G332" t="inlineStr">
         <is>
           <t>nectar</t>
         </is>
@@ -6600,10 +5536,7 @@
       <c r="C333">
         <v>7.05</v>
       </c>
-      <c r="F333">
-        <v>7.05</v>
-      </c>
-      <c r="H333" t="inlineStr">
+      <c r="G333" t="inlineStr">
         <is>
           <t>defeat</t>
         </is>
@@ -6618,10 +5551,7 @@
       <c r="C334">
         <v>7.05</v>
       </c>
-      <c r="F334">
-        <v>7.05</v>
-      </c>
-      <c r="H334" t="inlineStr">
+      <c r="G334" t="inlineStr">
         <is>
           <t>donation</t>
         </is>
@@ -6636,10 +5566,7 @@
       <c r="C335">
         <v>7.05</v>
       </c>
-      <c r="F335">
-        <v>7.05</v>
-      </c>
-      <c r="H335" t="inlineStr">
+      <c r="G335" t="inlineStr">
         <is>
           <t>vigilant</t>
         </is>
@@ -6654,10 +5581,7 @@
       <c r="C336">
         <v>7.06</v>
       </c>
-      <c r="F336">
-        <v>7.06</v>
-      </c>
-      <c r="H336" t="inlineStr">
+      <c r="G336" t="inlineStr">
         <is>
           <t>careful</t>
         </is>
@@ -6672,10 +5596,7 @@
       <c r="C337">
         <v>7.06</v>
       </c>
-      <c r="F337">
-        <v>7.06</v>
-      </c>
-      <c r="H337" t="inlineStr">
+      <c r="G337" t="inlineStr">
         <is>
           <t>ravishing</t>
         </is>
@@ -6690,10 +5611,7 @@
       <c r="C338">
         <v>7.06</v>
       </c>
-      <c r="F338">
-        <v>7.06</v>
-      </c>
-      <c r="H338" t="inlineStr">
+      <c r="G338" t="inlineStr">
         <is>
           <t>pressure</t>
         </is>
@@ -6708,10 +5626,7 @@
       <c r="C339">
         <v>7.06</v>
       </c>
-      <c r="F339">
-        <v>7.06</v>
-      </c>
-      <c r="H339" t="inlineStr">
+      <c r="G339" t="inlineStr">
         <is>
           <t>millionaire</t>
         </is>
@@ -6726,10 +5641,7 @@
       <c r="C340">
         <v>7.06</v>
       </c>
-      <c r="F340">
-        <v>7.06</v>
-      </c>
-      <c r="H340" t="inlineStr">
+      <c r="G340" t="inlineStr">
         <is>
           <t>preach</t>
         </is>
@@ -6744,10 +5656,7 @@
       <c r="C341">
         <v>7.06</v>
       </c>
-      <c r="F341">
-        <v>7.06</v>
-      </c>
-      <c r="H341" t="inlineStr">
+      <c r="G341" t="inlineStr">
         <is>
           <t>return</t>
         </is>
@@ -6762,10 +5671,7 @@
       <c r="C342">
         <v>7.06</v>
       </c>
-      <c r="F342">
-        <v>7.06</v>
-      </c>
-      <c r="H342" t="inlineStr">
+      <c r="G342" t="inlineStr">
         <is>
           <t>scoundrel</t>
         </is>
@@ -6780,10 +5686,7 @@
       <c r="C343">
         <v>7.06</v>
       </c>
-      <c r="F343">
-        <v>7.06</v>
-      </c>
-      <c r="H343" t="inlineStr">
+      <c r="G343" t="inlineStr">
         <is>
           <t>separation</t>
         </is>
@@ -6798,10 +5701,7 @@
       <c r="C344">
         <v>7.06</v>
       </c>
-      <c r="F344">
-        <v>7.06</v>
-      </c>
-      <c r="H344" t="inlineStr">
+      <c r="G344" t="inlineStr">
         <is>
           <t>orphan</t>
         </is>
@@ -6816,10 +5716,7 @@
       <c r="C345">
         <v>7.06</v>
       </c>
-      <c r="F345">
-        <v>7.06</v>
-      </c>
-      <c r="H345" t="inlineStr">
+      <c r="G345" t="inlineStr">
         <is>
           <t>waterproof</t>
         </is>

</xml_diff>